<commit_message>
Runs and data holding
</commit_message>
<xml_diff>
--- a/Archive/ABM Runs.xlsx
+++ b/Archive/ABM Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginab\Box\New Computer\Auburn\Data\ComplexModel_ABM\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4AC61C-DCE5-4559-8728-BE29ACB062E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D906C62-F87C-4CBB-B244-88A74D8A2606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="456" windowWidth="17304" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31200" yWindow="2400" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="97">
   <si>
     <t>ABM_run.10.12.22_b_</t>
   </si>
@@ -301,12 +301,6 @@
   </si>
   <si>
     <t>390838:390857</t>
-  </si>
-  <si>
-    <t>next thing to change: crash intensity -- crash to 50 indv; consider if pulses should be changed then or not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Might need to have a zero mig per generation for each of the different starting heterozygosities. </t>
   </si>
   <si>
     <t>add life history (consider specific species- reintroduction programs) – OR 1 sp with somewhat different changes in values (krat stuff but instead, they die earlier or mature later)</t>
@@ -366,12 +360,27 @@
   <si>
     <t>put the varying parameter sets in Cover.R rather than needing to manually change all the time</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">next thing to change: crash intensity -- crash to 50 indv; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>consider if pulses should be changed then or not</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +405,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -721,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2244,6 +2260,15 @@
       <c r="C25" t="s">
         <v>84</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G25" t="s">
         <v>32</v>
       </c>
@@ -2297,6 +2322,15 @@
       <c r="C26" t="s">
         <v>86</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G26" t="s">
         <v>32</v>
       </c>
@@ -2345,17 +2379,17 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="3" t="s">
+    <row r="31" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D31" s="3" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
@@ -2365,7 +2399,7 @@
     </row>
     <row r="33" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -2375,22 +2409,17 @@
     </row>
     <row r="35" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D35" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D38" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add rep succ data
</commit_message>
<xml_diff>
--- a/Archive/ABM Runs.xlsx
+++ b/Archive/ABM Runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginab\Box\New Computer\Auburn\Data\ComplexModel_ABM\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D906C62-F87C-4CBB-B244-88A74D8A2606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40959102-2915-4617-8645-A62057BE83F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31200" yWindow="2400" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={CFC0881D-C570-4D60-B8C1-048EFA885EF5}</author>
+  </authors>
+  <commentList>
+    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{CFC0881D-C570-4D60-B8C1-048EFA885EF5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duration for 100 years</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="104">
   <si>
     <t>ABM_run.10.12.22_b_</t>
   </si>
@@ -51,9 +69,6 @@
   </si>
   <si>
     <t>pop</t>
-  </si>
-  <si>
-    <t>deltaK</t>
   </si>
   <si>
     <t>k</t>
@@ -375,12 +390,36 @@
       <t>consider if pulses should be changed then or not</t>
     </r>
   </si>
+  <si>
+    <t>ABM_rub.12.5.22_0b</t>
+  </si>
+  <si>
+    <t>dropK</t>
+  </si>
+  <si>
+    <t>ABM_rub.12.5.22_0c</t>
+  </si>
+  <si>
+    <t>goal is to try and get the pop to crash!</t>
+  </si>
+  <si>
+    <t>401924:401943</t>
+  </si>
+  <si>
+    <t>same as above with greater duration; goal is to try and get the pop to crash!</t>
+  </si>
+  <si>
+    <t>401959:401978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO FAR, I have added miggy and sourcehet in Cover.R but did NOT put them in RunModel or as a parameter set. This will probs need some checks before running. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,8 +455,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,6 +488,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -449,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -457,6 +515,9 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,6 +533,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Gina Lamka" id="{D651F15D-83BA-4EB7-94FE-80E180A01DF5}" userId="Gina Lamka" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,12 +802,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J29" dT="2022-12-05T20:48:35.11" personId="{D651F15D-83BA-4EB7-94FE-80E180A01DF5}" id="{CFC0881D-C570-4D60-B8C1-048EFA885EF5}">
+    <text>Duration for 100 years</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,46 +839,46 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -811,25 +886,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K2">
         <v>500</v>
@@ -864,28 +939,28 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K3">
         <v>500</v>
@@ -920,28 +995,28 @@
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K4" s="2">
         <v>500</v>
@@ -976,34 +1051,34 @@
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K5" s="1">
         <v>500</v>
@@ -1036,39 +1111,39 @@
         <v>0</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
       <c r="J6" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K6" s="1">
         <v>500</v>
@@ -1101,39 +1176,39 @@
         <v>0</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
       </c>
       <c r="J7" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K7" s="1">
         <v>500</v>
@@ -1166,39 +1241,39 @@
         <v>0</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
       </c>
       <c r="J8" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K8" s="1">
         <v>500</v>
@@ -1231,39 +1306,39 @@
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
       <c r="J9" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K9" s="1">
         <v>500</v>
@@ -1296,39 +1371,39 @@
         <v>0</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
       </c>
       <c r="J10" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K10" s="1">
         <v>500</v>
@@ -1361,39 +1436,39 @@
         <v>0</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K11" s="1">
         <v>500</v>
@@ -1426,39 +1501,39 @@
         <v>0</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K12" s="1">
         <v>500</v>
@@ -1491,39 +1566,39 @@
         <v>0</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K13" s="1">
         <v>500</v>
@@ -1556,39 +1631,39 @@
         <v>0</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K14" s="1">
         <v>500</v>
@@ -1621,39 +1696,39 @@
         <v>0</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
       </c>
       <c r="J15" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K15" s="1">
         <v>500</v>
@@ -1686,39 +1761,39 @@
         <v>0</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
       </c>
       <c r="J16" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K16" s="1">
         <v>500</v>
@@ -1751,39 +1826,39 @@
         <v>0</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
       <c r="J17" s="1">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K17" s="1">
         <v>500</v>
@@ -1816,36 +1891,36 @@
         <v>0</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="2">
         <v>1</v>
       </c>
       <c r="J18" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K18" s="2">
         <v>500</v>
@@ -1878,36 +1953,36 @@
         <v>0</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
       </c>
       <c r="J19" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K19" s="2">
         <v>500</v>
@@ -1940,36 +2015,36 @@
         <v>0</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I20" s="2">
         <v>1</v>
       </c>
       <c r="J20" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K20" s="2">
         <v>500</v>
@@ -2002,36 +2077,36 @@
         <v>0</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2">
         <v>1</v>
       </c>
       <c r="J21" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K21" s="2">
         <v>500</v>
@@ -2064,36 +2139,36 @@
         <v>0</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
       </c>
       <c r="J22" s="2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K22" s="2">
         <v>500</v>
@@ -2126,36 +2201,36 @@
         <v>0</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K23">
         <v>500</v>
@@ -2188,36 +2263,36 @@
         <v>0</v>
       </c>
       <c r="U23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K24">
         <v>500</v>
@@ -2250,36 +2325,36 @@
         <v>0</v>
       </c>
       <c r="U24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K25">
         <v>500</v>
@@ -2312,36 +2387,36 @@
         <v>0</v>
       </c>
       <c r="U25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K26">
         <v>500</v>
@@ -2374,57 +2449,113 @@
         <v>0</v>
       </c>
       <c r="U26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D32" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D33" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D34" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D35" s="3" t="s">
-        <v>93</v>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="6">
+        <v>50</v>
+      </c>
+      <c r="P28" s="6">
+        <v>350</v>
+      </c>
+      <c r="U28" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="7">
+        <v>50</v>
+      </c>
+      <c r="P29" s="6">
+        <v>350</v>
+      </c>
+      <c r="U29" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="4:4" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D36" s="3" t="s">
-        <v>94</v>
+      <c r="D36" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D38" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D39" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D40" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D41" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D42" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D43" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data and run
</commit_message>
<xml_diff>
--- a/Archive/ABM Runs.xlsx
+++ b/Archive/ABM Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginab\Box\New Computer\Auburn\Data\ComplexModel_ABM\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95BA160-EE62-4810-B060-49BB8A9F795A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B6681-76BF-48E0-B25E-A2DB63315F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33435" yWindow="2730" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="148">
   <si>
     <t>ABM_run.10.12.22_b_</t>
   </si>
@@ -570,9 +570,6 @@
     <t>ABM_run.1.11.23_B</t>
   </si>
   <si>
-    <t>given 5000M mem</t>
-  </si>
-  <si>
     <t>434241:434260</t>
   </si>
   <si>
@@ -582,9 +579,6 @@
     <t>.45, 0.07</t>
   </si>
   <si>
-    <t>given 7500M</t>
-  </si>
-  <si>
     <t>436053:436072</t>
   </si>
   <si>
@@ -595,13 +589,22 @@
   </si>
   <si>
     <t>as of 1.13.23, rep success includes migrants in years, because I cahnged year born to the year they entered the pop. There are now measures for just migrants too tho.</t>
+  </si>
+  <si>
+    <t>given 7500M; 25 parameter sets</t>
+  </si>
+  <si>
+    <t>given 5000M mem; 8 parameter sets</t>
+  </si>
+  <si>
+    <t>next, change fecundity and max age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +676,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -701,13 +710,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -738,10 +747,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,8 +1062,8 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3092,7 +3103,7 @@
         <v>16</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>16</v>
@@ -3106,7 +3117,7 @@
       <c r="J36">
         <v>1</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="13">
         <v>300</v>
       </c>
       <c r="L36">
@@ -3148,13 +3159,25 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="12" t="s">
         <v>137</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H37" t="s">
         <v>122</v>
@@ -3206,13 +3229,13 @@
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="12" t="s">
         <v>130</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -3222,7 +3245,7 @@
         <v>16</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>16</v>
@@ -3236,7 +3259,7 @@
       <c r="J38">
         <v>1</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="13">
         <v>700</v>
       </c>
       <c r="L38">
@@ -3293,7 +3316,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>16</v>
@@ -3307,7 +3330,7 @@
       <c r="J39">
         <v>1</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="13">
         <v>100</v>
       </c>
       <c r="L39">
@@ -3349,19 +3372,19 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H40" t="s">
         <v>122</v>
       </c>
       <c r="I40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -3394,7 +3417,7 @@
         <v>350</v>
       </c>
       <c r="T40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U40">
         <v>5.5555555555555601E-2</v>
@@ -3406,14 +3429,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="K41" s="12"/>
+    <row r="41" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C43" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C46" t="s">

</xml_diff>

<commit_message>
clean up and add better notes
</commit_message>
<xml_diff>
--- a/Archive/ABM Runs.xlsx
+++ b/Archive/ABM Runs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginab\Box\New Computer\Auburn\Data\ComplexModel_ABM\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A82128-DD6B-4153-83DF-34F124E06636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33977003-A0F0-454B-90E6-CF23BE618156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,6 +56,18 @@
     <author>tc={D37EF45E-1776-45C7-A686-231D3B3CF349}</author>
     <author>tc={9589ABAC-6157-4ED5-860F-6CD8BF271430}</author>
     <author>tc={EF425E74-64E7-4C89-9CBB-3E45E4A7FD5C}</author>
+    <author>tc={82C90A01-84AF-4C4A-B4E4-684A58E7DDF1}</author>
+    <author>tc={C4FB2540-82E6-4D33-BA81-80975C9086D1}</author>
+    <author>tc={D0A3207F-FEEC-4794-AB42-0CEDFDFF8F90}</author>
+    <author>tc={8FC32205-512B-46C7-89A5-0E1ADF11CB1F}</author>
+    <author>tc={4AB27585-BD80-4D6C-8BDD-8322D2637174}</author>
+    <author>tc={50C1E468-3FE3-4425-AF63-F693B778E1EB}</author>
+    <author>tc={9B2957F2-B0F0-4676-938E-589BF91EDDDB}</author>
+    <author>tc={8297EA8D-E880-4ED0-B636-0A3BAE761372}</author>
+    <author>tc={1A7E678B-791B-4624-9617-45050294B705}</author>
+    <author>tc={C8B45157-0C7D-4F43-8981-E394CFA9B30A}</author>
+    <author>tc={43182A03-EEEB-49F0-BA20-619E7651014A}</author>
+    <author>tc={A126A3DF-DFE8-44DC-A108-85EC9F636C8F}</author>
   </authors>
   <commentList>
     <comment ref="L29" authorId="0" shapeId="0" xr:uid="{CFC0881D-C570-4D60-B8C1-048EFA885EF5}">
@@ -254,12 +266,168 @@
 f= 25 @ y=125, 140, 155, 170</t>
       </text>
     </comment>
+    <comment ref="H130" authorId="18" shapeId="0" xr:uid="{82C90A01-84AF-4C4A-B4E4-684A58E7DDF1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H131" authorId="19" shapeId="0" xr:uid="{C4FB2540-82E6-4D33-BA81-80975C9086D1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H132" authorId="20" shapeId="0" xr:uid="{D0A3207F-FEEC-4794-AB42-0CEDFDFF8F90}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H133" authorId="21" shapeId="0" xr:uid="{8FC32205-512B-46C7-89A5-0E1ADF11CB1F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H134" authorId="22" shapeId="0" xr:uid="{4AB27585-BD80-4D6C-8BDD-8322D2637174}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H135" authorId="23" shapeId="0" xr:uid="{50C1E468-3FE3-4425-AF63-F693B778E1EB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H136" authorId="24" shapeId="0" xr:uid="{9B2957F2-B0F0-4676-938E-589BF91EDDDB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H137" authorId="25" shapeId="0" xr:uid="{8297EA8D-E880-4ED0-B636-0A3BAE761372}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H138" authorId="26" shapeId="0" xr:uid="{1A7E678B-791B-4624-9617-45050294B705}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H139" authorId="27" shapeId="0" xr:uid="{C8B45157-0C7D-4F43-8981-E394CFA9B30A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H140" authorId="28" shapeId="0" xr:uid="{43182A03-EEEB-49F0-BA20-619E7651014A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H141" authorId="29" shapeId="0" xr:uid="{A126A3DF-DFE8-44DC-A108-85EC9F636C8F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="428">
   <si>
     <t>ABM_run.10.12.22_b_</t>
   </si>
@@ -1520,6 +1688,93 @@
   </si>
   <si>
     <t>615433:615452</t>
+  </si>
+  <si>
+    <t>final runs but ran more split for time sake</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>633956:633975</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3f</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3e</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>634176:634195</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3d</t>
+  </si>
+  <si>
+    <t>634196:634215</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3c</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>634216:634235</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3b</t>
+  </si>
+  <si>
+    <t>634257:634276</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL3a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_1LL30</t>
+  </si>
+  <si>
+    <t>634277:634296</t>
+  </si>
+  <si>
+    <t>634297:634316</t>
+  </si>
+  <si>
+    <t>0,a</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_2HL30a</t>
+  </si>
+  <si>
+    <t>634317:634336</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_2HH30a</t>
+  </si>
+  <si>
+    <t>634337:634356</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_2LL50a</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_2LL70a</t>
+  </si>
+  <si>
+    <t>fin_5.10.23_2LL10a</t>
+  </si>
+  <si>
+    <t>CANCELED due to being over max walltime</t>
   </si>
 </sst>
 </file>
@@ -1625,7 +1880,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2158,16 +2413,112 @@
 e= 100 @ y=125
 f= 25 @ y=125, 140, 155, 170</text>
   </threadedComment>
+  <threadedComment ref="H130" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{82C90A01-84AF-4C4A-B4E4-684A58E7DDF1}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H131" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{C4FB2540-82E6-4D33-BA81-80975C9086D1}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H132" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{D0A3207F-FEEC-4794-AB42-0CEDFDFF8F90}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H133" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{8FC32205-512B-46C7-89A5-0E1ADF11CB1F}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H134" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{4AB27585-BD80-4D6C-8BDD-8322D2637174}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H135" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{50C1E468-3FE3-4425-AF63-F693B778E1EB}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H136" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{9B2957F2-B0F0-4676-938E-589BF91EDDDB}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H137" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{8297EA8D-E880-4ED0-B636-0A3BAE761372}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H138" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{1A7E678B-791B-4624-9617-45050294B705}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H139" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{C8B45157-0C7D-4F43-8981-E394CFA9B30A}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H140" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{43182A03-EEEB-49F0-BA20-619E7651014A}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H141" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{A126A3DF-DFE8-44DC-A108-85EC9F636C8F}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA172"/>
+  <dimension ref="A1:AA193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10205,7 +10556,10 @@
       </c>
     </row>
     <row r="128" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
+      <c r="A128" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B128" s="9" t="s">
         <v>398</v>
       </c>
       <c r="C128" t="s">
@@ -10269,174 +10623,950 @@
         <v>384</v>
       </c>
     </row>
-    <row r="134" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C129" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="130" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>401</v>
+      </c>
+      <c r="C130" t="s">
+        <v>402</v>
+      </c>
+      <c r="H130" t="s">
+        <v>400</v>
+      </c>
+      <c r="I130">
+        <v>0.05</v>
+      </c>
+      <c r="J130">
+        <v>0.05</v>
+      </c>
+      <c r="K130">
+        <v>5</v>
+      </c>
+      <c r="L130">
+        <v>300</v>
+      </c>
+      <c r="M130">
+        <v>1000</v>
+      </c>
+      <c r="N130">
+        <v>1000</v>
+      </c>
+      <c r="O130">
+        <v>10</v>
+      </c>
+      <c r="P130">
+        <v>40</v>
+      </c>
+      <c r="Q130">
+        <v>9</v>
+      </c>
+      <c r="R130">
+        <v>2</v>
+      </c>
+      <c r="S130">
+        <v>1</v>
+      </c>
+      <c r="T130">
+        <v>350</v>
+      </c>
+      <c r="U130">
+        <v>1</v>
+      </c>
+      <c r="W130">
+        <v>100</v>
+      </c>
+      <c r="X130">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z130" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA130" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="131" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>405</v>
+      </c>
+      <c r="C131" t="s">
+        <v>403</v>
+      </c>
+      <c r="H131" t="s">
+        <v>404</v>
+      </c>
+      <c r="I131">
+        <v>0.05</v>
+      </c>
+      <c r="J131">
+        <v>0.05</v>
+      </c>
+      <c r="K131">
+        <v>5</v>
+      </c>
+      <c r="L131">
+        <v>300</v>
+      </c>
+      <c r="M131">
+        <v>1000</v>
+      </c>
+      <c r="N131">
+        <v>1000</v>
+      </c>
+      <c r="O131">
+        <v>10</v>
+      </c>
+      <c r="P131">
+        <v>40</v>
+      </c>
+      <c r="Q131">
+        <v>9</v>
+      </c>
+      <c r="R131">
+        <v>2</v>
+      </c>
+      <c r="S131">
+        <v>1</v>
+      </c>
+      <c r="T131">
+        <v>350</v>
+      </c>
+      <c r="U131">
+        <v>1</v>
+      </c>
+      <c r="W131">
+        <v>100</v>
+      </c>
+      <c r="X131">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z131" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="132" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>407</v>
+      </c>
+      <c r="C132" t="s">
+        <v>406</v>
+      </c>
+      <c r="H132" t="s">
+        <v>408</v>
+      </c>
+      <c r="I132">
+        <v>0.05</v>
+      </c>
+      <c r="J132">
+        <v>0.05</v>
+      </c>
+      <c r="K132">
+        <v>5</v>
+      </c>
+      <c r="L132">
+        <v>300</v>
+      </c>
+      <c r="M132">
+        <v>1000</v>
+      </c>
+      <c r="N132">
+        <v>1000</v>
+      </c>
+      <c r="O132">
+        <v>10</v>
+      </c>
+      <c r="P132">
+        <v>40</v>
+      </c>
+      <c r="Q132">
+        <v>9</v>
+      </c>
+      <c r="R132">
+        <v>2</v>
+      </c>
+      <c r="S132">
+        <v>1</v>
+      </c>
+      <c r="T132">
+        <v>350</v>
+      </c>
+      <c r="U132">
+        <v>1</v>
+      </c>
+      <c r="W132">
+        <v>100</v>
+      </c>
+      <c r="X132">
+        <v>0</v>
+      </c>
+      <c r="Y132" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA132" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="133" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>411</v>
+      </c>
+      <c r="C133" t="s">
+        <v>409</v>
+      </c>
+      <c r="H133" t="s">
+        <v>410</v>
+      </c>
+      <c r="I133">
+        <v>0.05</v>
+      </c>
+      <c r="J133">
+        <v>0.05</v>
+      </c>
+      <c r="K133">
+        <v>5</v>
+      </c>
+      <c r="L133">
+        <v>300</v>
+      </c>
+      <c r="M133">
+        <v>1000</v>
+      </c>
+      <c r="N133">
+        <v>1000</v>
+      </c>
+      <c r="O133">
+        <v>10</v>
+      </c>
+      <c r="P133">
+        <v>40</v>
+      </c>
+      <c r="Q133">
+        <v>9</v>
+      </c>
+      <c r="R133">
+        <v>2</v>
+      </c>
+      <c r="S133">
+        <v>1</v>
+      </c>
+      <c r="T133">
+        <v>350</v>
+      </c>
+      <c r="U133">
+        <v>1</v>
+      </c>
+      <c r="W133">
+        <v>100</v>
+      </c>
+      <c r="X133">
+        <v>0</v>
+      </c>
+      <c r="Y133" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z133" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA133" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="134" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>413</v>
+      </c>
       <c r="C134" t="s">
+        <v>412</v>
+      </c>
+      <c r="H134" t="s">
+        <v>415</v>
+      </c>
+      <c r="I134">
+        <v>0.05</v>
+      </c>
+      <c r="J134">
+        <v>0.05</v>
+      </c>
+      <c r="K134">
+        <v>5</v>
+      </c>
+      <c r="L134">
+        <v>300</v>
+      </c>
+      <c r="M134">
+        <v>1000</v>
+      </c>
+      <c r="N134">
+        <v>1000</v>
+      </c>
+      <c r="O134">
+        <v>10</v>
+      </c>
+      <c r="P134">
+        <v>40</v>
+      </c>
+      <c r="Q134">
+        <v>9</v>
+      </c>
+      <c r="R134">
+        <v>2</v>
+      </c>
+      <c r="S134">
+        <v>1</v>
+      </c>
+      <c r="T134">
+        <v>350</v>
+      </c>
+      <c r="U134">
+        <v>1</v>
+      </c>
+      <c r="W134">
+        <v>100</v>
+      </c>
+      <c r="X134">
+        <v>0</v>
+      </c>
+      <c r="Y134" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z134" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA134" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="135" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>417</v>
+      </c>
+      <c r="C135" t="s">
+        <v>414</v>
+      </c>
+      <c r="H135" t="s">
+        <v>296</v>
+      </c>
+      <c r="I135">
+        <v>0.05</v>
+      </c>
+      <c r="J135">
+        <v>0.05</v>
+      </c>
+      <c r="K135">
+        <v>5</v>
+      </c>
+      <c r="L135">
+        <v>300</v>
+      </c>
+      <c r="M135">
+        <v>1000</v>
+      </c>
+      <c r="N135">
+        <v>1000</v>
+      </c>
+      <c r="O135">
+        <v>10</v>
+      </c>
+      <c r="P135">
+        <v>40</v>
+      </c>
+      <c r="Q135">
+        <v>9</v>
+      </c>
+      <c r="R135">
+        <v>2</v>
+      </c>
+      <c r="S135">
+        <v>1</v>
+      </c>
+      <c r="T135">
+        <v>350</v>
+      </c>
+      <c r="U135">
+        <v>1</v>
+      </c>
+      <c r="W135">
+        <v>100</v>
+      </c>
+      <c r="X135">
+        <v>0</v>
+      </c>
+      <c r="Y135" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z135" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA135" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="136" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>418</v>
+      </c>
+      <c r="C136" t="s">
+        <v>416</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136">
+        <v>0.05</v>
+      </c>
+      <c r="J136">
+        <v>0.05</v>
+      </c>
+      <c r="K136">
+        <v>5</v>
+      </c>
+      <c r="L136">
+        <v>300</v>
+      </c>
+      <c r="M136">
+        <v>1000</v>
+      </c>
+      <c r="N136">
+        <v>1000</v>
+      </c>
+      <c r="O136">
+        <v>10</v>
+      </c>
+      <c r="P136">
+        <v>40</v>
+      </c>
+      <c r="Q136">
+        <v>9</v>
+      </c>
+      <c r="R136">
+        <v>2</v>
+      </c>
+      <c r="S136">
+        <v>1</v>
+      </c>
+      <c r="T136">
+        <v>350</v>
+      </c>
+      <c r="U136">
+        <v>1</v>
+      </c>
+      <c r="W136">
+        <v>100</v>
+      </c>
+      <c r="X136">
+        <v>0</v>
+      </c>
+      <c r="Y136" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z136" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA136" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="137" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>421</v>
+      </c>
+      <c r="C137" t="s">
+        <v>420</v>
+      </c>
+      <c r="H137" t="s">
+        <v>419</v>
+      </c>
+      <c r="I137">
+        <v>0.4</v>
+      </c>
+      <c r="J137">
+        <v>0.05</v>
+      </c>
+      <c r="K137">
+        <v>5</v>
+      </c>
+      <c r="L137">
+        <v>300</v>
+      </c>
+      <c r="M137">
+        <v>1000</v>
+      </c>
+      <c r="N137">
+        <v>1000</v>
+      </c>
+      <c r="O137">
+        <v>10</v>
+      </c>
+      <c r="P137">
+        <v>40</v>
+      </c>
+      <c r="Q137">
+        <v>9</v>
+      </c>
+      <c r="R137">
+        <v>2</v>
+      </c>
+      <c r="S137">
+        <v>1</v>
+      </c>
+      <c r="T137">
+        <v>350</v>
+      </c>
+      <c r="U137">
+        <v>1</v>
+      </c>
+      <c r="W137">
+        <v>100</v>
+      </c>
+      <c r="X137">
+        <v>0</v>
+      </c>
+      <c r="Y137" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z137" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA137" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="138" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>423</v>
+      </c>
+      <c r="C138" t="s">
+        <v>422</v>
+      </c>
+      <c r="H138" t="s">
+        <v>419</v>
+      </c>
+      <c r="I138">
+        <v>0.4</v>
+      </c>
+      <c r="J138">
+        <v>0.4</v>
+      </c>
+      <c r="K138">
+        <v>5</v>
+      </c>
+      <c r="L138">
+        <v>300</v>
+      </c>
+      <c r="M138">
+        <v>1000</v>
+      </c>
+      <c r="N138">
+        <v>1000</v>
+      </c>
+      <c r="O138">
+        <v>10</v>
+      </c>
+      <c r="P138">
+        <v>40</v>
+      </c>
+      <c r="Q138">
+        <v>9</v>
+      </c>
+      <c r="R138">
+        <v>2</v>
+      </c>
+      <c r="S138">
+        <v>1</v>
+      </c>
+      <c r="T138">
+        <v>350</v>
+      </c>
+      <c r="U138">
+        <v>1</v>
+      </c>
+      <c r="W138">
+        <v>100</v>
+      </c>
+      <c r="X138">
+        <v>0</v>
+      </c>
+      <c r="Y138" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z138" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA138" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="139" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="C139" t="s">
+        <v>424</v>
+      </c>
+      <c r="H139" t="s">
+        <v>419</v>
+      </c>
+      <c r="I139">
+        <v>0.05</v>
+      </c>
+      <c r="J139">
+        <v>0.05</v>
+      </c>
+      <c r="K139">
+        <v>5</v>
+      </c>
+      <c r="L139">
+        <v>500</v>
+      </c>
+      <c r="M139">
+        <v>1000</v>
+      </c>
+      <c r="N139">
+        <v>1000</v>
+      </c>
+      <c r="O139">
+        <v>10</v>
+      </c>
+      <c r="P139">
+        <v>40</v>
+      </c>
+      <c r="Q139">
+        <v>9</v>
+      </c>
+      <c r="R139">
+        <v>2</v>
+      </c>
+      <c r="S139">
+        <v>1</v>
+      </c>
+      <c r="T139">
+        <v>350</v>
+      </c>
+      <c r="U139">
+        <v>1</v>
+      </c>
+      <c r="W139">
+        <v>100</v>
+      </c>
+      <c r="X139">
+        <v>0</v>
+      </c>
+      <c r="Y139" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z139" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA139" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="140" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="C140" t="s">
+        <v>425</v>
+      </c>
+      <c r="H140" t="s">
+        <v>419</v>
+      </c>
+      <c r="I140">
+        <v>0.05</v>
+      </c>
+      <c r="J140">
+        <v>0.05</v>
+      </c>
+      <c r="K140">
+        <v>5</v>
+      </c>
+      <c r="L140">
+        <v>700</v>
+      </c>
+      <c r="M140">
+        <v>1000</v>
+      </c>
+      <c r="N140">
+        <v>1000</v>
+      </c>
+      <c r="O140">
+        <v>10</v>
+      </c>
+      <c r="P140">
+        <v>40</v>
+      </c>
+      <c r="Q140">
+        <v>9</v>
+      </c>
+      <c r="R140">
+        <v>2</v>
+      </c>
+      <c r="S140">
+        <v>1</v>
+      </c>
+      <c r="T140">
+        <v>350</v>
+      </c>
+      <c r="U140">
+        <v>1</v>
+      </c>
+      <c r="W140">
+        <v>100</v>
+      </c>
+      <c r="X140">
+        <v>0</v>
+      </c>
+      <c r="Y140" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z140" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA140" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="141" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="C141" t="s">
+        <v>426</v>
+      </c>
+      <c r="H141" t="s">
+        <v>419</v>
+      </c>
+      <c r="I141">
+        <v>0.05</v>
+      </c>
+      <c r="J141">
+        <v>0.05</v>
+      </c>
+      <c r="K141">
+        <v>5</v>
+      </c>
+      <c r="L141">
+        <v>100</v>
+      </c>
+      <c r="M141">
+        <v>1000</v>
+      </c>
+      <c r="N141">
+        <v>1000</v>
+      </c>
+      <c r="O141">
+        <v>10</v>
+      </c>
+      <c r="P141">
+        <v>40</v>
+      </c>
+      <c r="Q141">
+        <v>9</v>
+      </c>
+      <c r="R141">
+        <v>2</v>
+      </c>
+      <c r="S141">
+        <v>1</v>
+      </c>
+      <c r="T141">
+        <v>350</v>
+      </c>
+      <c r="U141">
+        <v>1</v>
+      </c>
+      <c r="W141">
+        <v>100</v>
+      </c>
+      <c r="X141">
+        <v>0</v>
+      </c>
+      <c r="Y141" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z141" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA141" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C155" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="135" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C135" t="s">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C136" s="21" t="s">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C157" s="21" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="137" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C137" t="s">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C158" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="141" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C141" t="s">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C162" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C143" t="s">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C164" t="s">
         <v>188</v>
       </c>
-      <c r="H143" t="s">
+      <c r="H164" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C144" t="s">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C165" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C145" s="20" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C166" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C146" t="s">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C167" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C147" t="s">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C168" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>227</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B169" t="s">
         <v>226</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C169" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C149" s="8" t="s">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C170" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C150" t="s">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C171" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C151" t="s">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C172" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C152" t="s">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C173" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C155" t="s">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C176" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C156" t="s">
+    <row r="177" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C177" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C157" t="s">
+    <row r="178" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C178" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C158" t="s">
+    <row r="179" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C179" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C159" t="s">
+    <row r="180" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C180" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C160" t="s">
+    <row r="181" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C181" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="162" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D162" s="6" t="s">
+    <row r="183" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D183" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D163" t="s">
+    <row r="184" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D184" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="164" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D164" s="7" t="s">
+    <row r="185" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D185" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="165" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D165" s="3" t="s">
+    <row r="186" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D186" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="166" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D166" s="3" t="s">
+    <row r="187" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D187" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D167" s="3" t="s">
+    <row r="188" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D188" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="168" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D168" s="3" t="s">
+    <row r="189" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D189" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="169" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D169" s="6" t="s">
+    <row r="190" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D190" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="170" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D170" s="3" t="s">
+    <row r="191" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D191" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="172" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D172" s="3" t="s">
+    <row r="193" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D193" s="3" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C136" r:id="rId1" display="https://www.natureserve.org/sites/default/files/publications/files/natureserveconservationstatusfactors_apr12.pdf" xr:uid="{0084F411-030C-4AB0-936F-5DA9CEBDCCC8}"/>
+    <hyperlink ref="C157" r:id="rId1" display="https://www.natureserve.org/sites/default/files/publications/files/natureserveconservationstatusfactors_apr12.pdf" xr:uid="{0084F411-030C-4AB0-936F-5DA9CEBDCCC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
update ReadMe and add data
</commit_message>
<xml_diff>
--- a/Archive/ABM Runs.xlsx
+++ b/Archive/ABM Runs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginab\Box\New Computer\Auburn\Data\ComplexModel_ABM\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477AED2F-0841-417D-A0CF-B6BF09E5A4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5179545F-E204-4337-9E93-9D4C91129D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,6 +99,46 @@
     <author>tc={8B36E44F-4EF7-40F9-8BB2-8F3851006A51}</author>
     <author>tc={B25E90D7-FF3C-4024-8C7B-EA52ACC26874}</author>
     <author>tc={D2984361-F13F-469B-B1E2-0127DBB65D87}</author>
+    <author>tc={3090656F-DDA7-467E-8B6F-8789C89F58CA}</author>
+    <author>tc={7B1500BC-F541-407D-97F0-6C0D03627AE1}</author>
+    <author>tc={BAA31817-EAC8-4F5E-BC03-46CBE1BE9228}</author>
+    <author>tc={2A6EDDAA-3111-42C7-8497-86E1B37E17FA}</author>
+    <author>tc={12DF5D79-A07E-481B-8E6E-70672A6B4324}</author>
+    <author>tc={F309F0DE-3199-4E63-A503-3A5DB1CCAE81}</author>
+    <author>tc={87F8F7F6-D6DF-4EAC-A492-BC4B01D175F4}</author>
+    <author>tc={DA037A73-0CEA-4466-9367-C518395BF34E}</author>
+    <author>tc={4355BEFD-D19F-4C0A-A9E0-892AB96FBA62}</author>
+    <author>tc={BBD32FE6-6008-44B1-800D-5FB543C5BD50}</author>
+    <author>tc={D11DEF16-3D72-4CA6-8ADD-398796FE16A8}</author>
+    <author>tc={8DBA1E78-F9D3-45D8-AFD5-E10CE4FAF0B9}</author>
+    <author>tc={FC7032BC-CE89-447D-88CA-C3CD2FB16213}</author>
+    <author>tc={256E817F-CF21-4C20-B0DE-95ECC78BA9D4}</author>
+    <author>tc={8C0C60CD-2FFC-416C-88D6-E4416022371E}</author>
+    <author>tc={5DE256C6-C31F-4605-A18D-2BE29D766566}</author>
+    <author>tc={A42173E6-84D0-46C7-B378-8634718C2FC8}</author>
+    <author>tc={EBF43E29-75DA-480E-BBE5-B12D156F4C90}</author>
+    <author>tc={6C977184-882A-441A-AE0B-68A20136A079}</author>
+    <author>tc={ED91EFEA-F400-49F6-85FB-42D020B71268}</author>
+    <author>tc={EBAC87DC-D6FE-4071-AAE6-0C36885047E2}</author>
+    <author>tc={8C4EA953-475C-4BBB-9B78-DAFADCFDBEFA}</author>
+    <author>tc={2FEBDDD9-921D-4287-8219-55D25EFC68AD}</author>
+    <author>tc={0E67955F-4ADE-4A4F-BAF9-F1899691263A}</author>
+    <author>tc={963825C3-BD84-4CE4-88BF-AA168CC7DAC9}</author>
+    <author>tc={44A9303A-88D5-4BB8-9879-72F5FB7F39F1}</author>
+    <author>tc={09306D4D-E8BF-4998-9564-E7BA359D5135}</author>
+    <author>tc={515314A8-BFD2-41C1-90E5-88B3BF915352}</author>
+    <author>tc={EBE5ABD0-D0E0-4D98-8775-45A40346A5B8}</author>
+    <author>tc={45EB5FC7-B067-4E16-BC88-2FE18DB32EE9}</author>
+    <author>tc={D7E8C1D8-0A1A-4552-9BE2-DF2C70622C4F}</author>
+    <author>tc={A6232F6B-D4D4-4C06-A077-77622943784A}</author>
+    <author>tc={202159C9-01FE-40D8-BC35-E4387FDA6974}</author>
+    <author>tc={48FED36A-64A0-4E6E-B2FC-4DCB941E833D}</author>
+    <author>tc={98B014DF-78D4-4975-90B9-78901C25281F}</author>
+    <author>tc={68770FB5-ABB7-45E1-969B-1AB4920C0364}</author>
+    <author>tc={96A288A9-00D2-44F1-81EB-075B4A2B779B}</author>
+    <author>tc={70261BF8-3B60-447F-82FE-F3F6F24265EF}</author>
+    <author>tc={D4B85581-504C-45FC-83BB-050D16433043}</author>
+    <author>tc={0CC2D386-04EA-4FB3-8FC0-C44B9D3B579B}</author>
   </authors>
   <commentList>
     <comment ref="L29" authorId="0" shapeId="0" xr:uid="{CFC0881D-C570-4D60-B8C1-048EFA885EF5}">
@@ -843,12 +884,522 @@
 f= 25 @ y=125, 140, 155, 170</t>
       </text>
     </comment>
+    <comment ref="H170" authorId="60" shapeId="0" xr:uid="{3090656F-DDA7-467E-8B6F-8789C89F58CA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H171" authorId="61" shapeId="0" xr:uid="{7B1500BC-F541-407D-97F0-6C0D03627AE1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H172" authorId="62" shapeId="0" xr:uid="{BAA31817-EAC8-4F5E-BC03-46CBE1BE9228}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H173" authorId="63" shapeId="0" xr:uid="{2A6EDDAA-3111-42C7-8497-86E1B37E17FA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H174" authorId="64" shapeId="0" xr:uid="{12DF5D79-A07E-481B-8E6E-70672A6B4324}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H175" authorId="65" shapeId="0" xr:uid="{F309F0DE-3199-4E63-A503-3A5DB1CCAE81}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H176" authorId="66" shapeId="0" xr:uid="{87F8F7F6-D6DF-4EAC-A492-BC4B01D175F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H177" authorId="67" shapeId="0" xr:uid="{DA037A73-0CEA-4466-9367-C518395BF34E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H178" authorId="68" shapeId="0" xr:uid="{4355BEFD-D19F-4C0A-A9E0-892AB96FBA62}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H179" authorId="69" shapeId="0" xr:uid="{BBD32FE6-6008-44B1-800D-5FB543C5BD50}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H180" authorId="70" shapeId="0" xr:uid="{D11DEF16-3D72-4CA6-8ADD-398796FE16A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H181" authorId="71" shapeId="0" xr:uid="{8DBA1E78-F9D3-45D8-AFD5-E10CE4FAF0B9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H182" authorId="72" shapeId="0" xr:uid="{FC7032BC-CE89-447D-88CA-C3CD2FB16213}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H183" authorId="73" shapeId="0" xr:uid="{256E817F-CF21-4C20-B0DE-95ECC78BA9D4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H184" authorId="74" shapeId="0" xr:uid="{8C0C60CD-2FFC-416C-88D6-E4416022371E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="B185" authorId="75" shapeId="0" xr:uid="{5DE256C6-C31F-4605-A18D-2BE29D766566}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    750890:750909 canceled due to mistype in runmodel.sh</t>
+      </text>
+    </comment>
+    <comment ref="H185" authorId="76" shapeId="0" xr:uid="{A42173E6-84D0-46C7-B378-8634718C2FC8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H186" authorId="77" shapeId="0" xr:uid="{EBF43E29-75DA-480E-BBE5-B12D156F4C90}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H187" authorId="78" shapeId="0" xr:uid="{6C977184-882A-441A-AE0B-68A20136A079}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H188" authorId="79" shapeId="0" xr:uid="{ED91EFEA-F400-49F6-85FB-42D020B71268}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H189" authorId="80" shapeId="0" xr:uid="{EBAC87DC-D6FE-4071-AAE6-0C36885047E2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H190" authorId="81" shapeId="0" xr:uid="{8C4EA953-475C-4BBB-9B78-DAFADCFDBEFA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H191" authorId="82" shapeId="0" xr:uid="{2FEBDDD9-921D-4287-8219-55D25EFC68AD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H192" authorId="83" shapeId="0" xr:uid="{0E67955F-4ADE-4A4F-BAF9-F1899691263A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H193" authorId="84" shapeId="0" xr:uid="{963825C3-BD84-4CE4-88BF-AA168CC7DAC9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H194" authorId="85" shapeId="0" xr:uid="{44A9303A-88D5-4BB8-9879-72F5FB7F39F1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H195" authorId="86" shapeId="0" xr:uid="{09306D4D-E8BF-4998-9564-E7BA359D5135}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H196" authorId="87" shapeId="0" xr:uid="{515314A8-BFD2-41C1-90E5-88B3BF915352}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="B197" authorId="88" shapeId="0" xr:uid="{EBE5ABD0-D0E0-4D98-8775-45A40346A5B8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    757600:757619 canceled due to mistype</t>
+      </text>
+    </comment>
+    <comment ref="H197" authorId="89" shapeId="0" xr:uid="{45EB5FC7-B067-4E16-BC88-2FE18DB32EE9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H198" authorId="90" shapeId="0" xr:uid="{D7E8C1D8-0A1A-4552-9BE2-DF2C70622C4F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H199" authorId="91" shapeId="0" xr:uid="{A6232F6B-D4D4-4C06-A077-77622943784A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H200" authorId="92" shapeId="0" xr:uid="{202159C9-01FE-40D8-BC35-E4387FDA6974}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H201" authorId="93" shapeId="0" xr:uid="{48FED36A-64A0-4E6E-B2FC-4DCB941E833D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H202" authorId="94" shapeId="0" xr:uid="{98B014DF-78D4-4975-90B9-78901C25281F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H203" authorId="95" shapeId="0" xr:uid="{68770FB5-ABB7-45E1-969B-1AB4920C0364}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H205" authorId="96" shapeId="0" xr:uid="{96A288A9-00D2-44F1-81EB-075B4A2B779B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H206" authorId="97" shapeId="0" xr:uid="{70261BF8-3B60-447F-82FE-F3F6F24265EF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H207" authorId="98" shapeId="0" xr:uid="{D4B85581-504C-45FC-83BB-050D16433043}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
+    <comment ref="H208" authorId="99" shapeId="0" xr:uid="{0CC2D386-04EA-4FB3-8FC0-C44B9D3B579B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="592">
   <si>
     <t>ABM_run.10.12.22_b_</t>
   </si>
@@ -2384,6 +2935,340 @@
   </si>
   <si>
     <t>671747:671751</t>
+  </si>
+  <si>
+    <t>fin_9.8.23_LL30m</t>
+  </si>
+  <si>
+    <t>fin_9.8.23_LL3am</t>
+  </si>
+  <si>
+    <t>mutate OFF</t>
+  </si>
+  <si>
+    <t>1 rep cuz of maintenance. Running to see if my mu is hella too high.</t>
+  </si>
+  <si>
+    <t>746572:746591</t>
+  </si>
+  <si>
+    <t>746592:746611</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL30</t>
+  </si>
+  <si>
+    <t>mu = 0.00000001</t>
+  </si>
+  <si>
+    <t>750441:750460</t>
+  </si>
+  <si>
+    <t>750461:750480</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3a</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3b</t>
+  </si>
+  <si>
+    <t>750481:750500</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3c</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3d</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3e</t>
+  </si>
+  <si>
+    <t>750504:750523</t>
+  </si>
+  <si>
+    <t>750525:750544</t>
+  </si>
+  <si>
+    <t>750546:750565</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3f</t>
+  </si>
+  <si>
+    <t>750570:750589</t>
+  </si>
+  <si>
+    <t>end_9.18.23_HH30</t>
+  </si>
+  <si>
+    <t>end_9.18.23_HH3a</t>
+  </si>
+  <si>
+    <t>750598:750617</t>
+  </si>
+  <si>
+    <t>750618:750637</t>
+  </si>
+  <si>
+    <t>end_9.18.23_HL30</t>
+  </si>
+  <si>
+    <t>end_9.18.23_HL3a</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LH30</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LH3a</t>
+  </si>
+  <si>
+    <t>750639:750658</t>
+  </si>
+  <si>
+    <t>750660:750679</t>
+  </si>
+  <si>
+    <t>750682:750701</t>
+  </si>
+  <si>
+    <t>750702:750721</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL10</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL1a</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL1b</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL1c</t>
+  </si>
+  <si>
+    <t>750849:750868</t>
+  </si>
+  <si>
+    <t>750870:750889</t>
+  </si>
+  <si>
+    <t>750910:750929</t>
+  </si>
+  <si>
+    <t>750931:750950</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL70</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL7a</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL7b</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL7c</t>
+  </si>
+  <si>
+    <t>750958:750977</t>
+  </si>
+  <si>
+    <t>750978:750997</t>
+  </si>
+  <si>
+    <t>750999:751018</t>
+  </si>
+  <si>
+    <t>751019:751038</t>
+  </si>
+  <si>
+    <t>end_9.18.23_nbtl3a</t>
+  </si>
+  <si>
+    <t>end_9.18.23_nbtl30</t>
+  </si>
+  <si>
+    <t>751040:751059</t>
+  </si>
+  <si>
+    <t>751060:751079</t>
+  </si>
+  <si>
+    <t>751087:751106</t>
+  </si>
+  <si>
+    <t>751107:751126</t>
+  </si>
+  <si>
+    <t>751127:751146</t>
+  </si>
+  <si>
+    <t>751149:751168</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3c.</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3b.</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL3a.</t>
+  </si>
+  <si>
+    <t>end_9.18.23_LL30.</t>
+  </si>
+  <si>
+    <t>end_9.27.23_LH3a</t>
+  </si>
+  <si>
+    <t>757622:757641</t>
+  </si>
+  <si>
+    <t>757652:757671</t>
+  </si>
+  <si>
+    <t>end_9.27.23_LH30</t>
+  </si>
+  <si>
+    <t>end_9.27.23_HL30</t>
+  </si>
+  <si>
+    <t>757672:757691</t>
+  </si>
+  <si>
+    <t>757692:757711</t>
+  </si>
+  <si>
+    <t>many failed</t>
+  </si>
+  <si>
+    <t>end_10.2.23_LL10</t>
+  </si>
+  <si>
+    <t>760212:760231</t>
+  </si>
+  <si>
+    <t>end_10.2.23_LL1b</t>
+  </si>
+  <si>
+    <t>end_10.2.23_LL1c</t>
+  </si>
+  <si>
+    <t>760233:760252</t>
+  </si>
+  <si>
+    <t>760254:760273</t>
+  </si>
+  <si>
+    <t>these next ones are just in case!</t>
+  </si>
+  <si>
+    <t>end_10.4.23_LL10</t>
+  </si>
+  <si>
+    <t>end_10.4.23_LL1b</t>
+  </si>
+  <si>
+    <t>end_10.4.23_LL1c</t>
+  </si>
+  <si>
+    <t>762162:762181</t>
+  </si>
+  <si>
+    <t>762182:762201</t>
+  </si>
+  <si>
+    <t>762203:762222</t>
+  </si>
+  <si>
+    <t>end_10.4.23_LL10c</t>
+  </si>
+  <si>
+    <t>762225:762244</t>
+  </si>
+  <si>
+    <t>end_9.27.23_HL3a</t>
+  </si>
+  <si>
+    <t>2, 5, 7, 8, 15, 19</t>
+  </si>
+  <si>
+    <t>1, 2, 5, 6, 7, 15</t>
+  </si>
+  <si>
+    <t>6, 13, 14, 17, 18, 19, 20</t>
+  </si>
+  <si>
+    <t>errors</t>
+  </si>
+  <si>
+    <t>[1] "The next generation's population size will be 18 K is 100 k is 1000"
+[1] "the number of offspring needed is 6"
+[1] "there are 3 babies added to the pop"
+[1] "killed 3 individuals"
+[1] "DONE! 132 param 1 rep 1"
+[1] "killed 0 individuals"
+[1] "the sex ratio is 0.75"
+[1] "there are 3 pairs"
+[1] "The next generation's population size will be 20 K is 100 k is 1000"
+[1] "the number of offspring needed is 8"
+[1] "there are 3 babies added to the pop"
+[1] "killed 2 individuals"
+[1] "DONE! 133 param 1 rep 1"
+[1] "killed 2 individuals"
+[1] "the sex ratio is 0.875"
+[1] "there are 1 pairs"
+[1] "The next generation's population size will be 11 K is 100 k is 1000"
+[1] "the number of offspring needed is 3"
+Error in parents[n, , drop = FALSE] : subscript out of bounds
+Calls: RunModel -&gt; Breed</t>
+  </si>
+  <si>
+    <t>[1] "The next generation's population size will be 20 K is 100 k is 1000"</t>
+  </si>
+  <si>
+    <t>[1] "the number of offspring needed is 5"</t>
+  </si>
+  <si>
+    <t>[1] "there are 3 babies added to the pop"</t>
+  </si>
+  <si>
+    <t>[1] "killed 4 individuals"</t>
+  </si>
+  <si>
+    <t>[1] "DONE! 125 param 1 rep 1"</t>
+  </si>
+  <si>
+    <t>[1] "Cleaning up dead!"</t>
+  </si>
+  <si>
+    <t>[1] "killed 0 individuals"</t>
+  </si>
+  <si>
+    <t>[1] "the sex ratio is 0.857142857142857"</t>
+  </si>
+  <si>
+    <t>[1] "there are 2 pairs"</t>
+  </si>
+  <si>
+    <t>[1] "the number of offspring needed is 6"</t>
+  </si>
+  <si>
+    <t>Error in parents[n, , drop = FALSE] : subscript out of bounds</t>
+  </si>
+  <si>
+    <t>Calls: RunModel -&gt; Breed</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 8, 10, 11, 12, 13, 16</t>
+  </si>
+  <si>
+    <t>6, 8, 9, 18, 19</t>
+  </si>
+  <si>
+    <t>3, 5, 6, 9, 16, 19, 20</t>
   </si>
 </sst>
 </file>
@@ -2500,7 +3385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2573,8 +3458,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2591,12 +3488,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2638,6 +3546,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3376,20 +4293,331 @@
 e= 100 @ y=125
 f= 25 @ y=125, 140, 155, 170</text>
   </threadedComment>
+  <threadedComment ref="H170" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{3090656F-DDA7-467E-8B6F-8789C89F58CA}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H171" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{7B1500BC-F541-407D-97F0-6C0D03627AE1}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H172" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{BAA31817-EAC8-4F5E-BC03-46CBE1BE9228}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H173" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{2A6EDDAA-3111-42C7-8497-86E1B37E17FA}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H174" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{12DF5D79-A07E-481B-8E6E-70672A6B4324}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H175" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{F309F0DE-3199-4E63-A503-3A5DB1CCAE81}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H176" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{87F8F7F6-D6DF-4EAC-A492-BC4B01D175F4}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H177" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{DA037A73-0CEA-4466-9367-C518395BF34E}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H178" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{4355BEFD-D19F-4C0A-A9E0-892AB96FBA62}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H179" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{BBD32FE6-6008-44B1-800D-5FB543C5BD50}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H180" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{D11DEF16-3D72-4CA6-8ADD-398796FE16A8}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H181" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{8DBA1E78-F9D3-45D8-AFD5-E10CE4FAF0B9}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H182" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{FC7032BC-CE89-447D-88CA-C3CD2FB16213}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H183" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{256E817F-CF21-4C20-B0DE-95ECC78BA9D4}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H184" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{8C0C60CD-2FFC-416C-88D6-E4416022371E}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="B185" dT="2023-09-18T19:52:21.26" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{5DE256C6-C31F-4605-A18D-2BE29D766566}">
+    <text>750890:750909 canceled due to mistype in runmodel.sh</text>
+  </threadedComment>
+  <threadedComment ref="H185" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{A42173E6-84D0-46C7-B378-8634718C2FC8}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H186" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{EBF43E29-75DA-480E-BBE5-B12D156F4C90}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H187" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{6C977184-882A-441A-AE0B-68A20136A079}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H188" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{ED91EFEA-F400-49F6-85FB-42D020B71268}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H189" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{EBAC87DC-D6FE-4071-AAE6-0C36885047E2}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H190" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{8C4EA953-475C-4BBB-9B78-DAFADCFDBEFA}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H191" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{2FEBDDD9-921D-4287-8219-55D25EFC68AD}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H192" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{0E67955F-4ADE-4A4F-BAF9-F1899691263A}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H193" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{963825C3-BD84-4CE4-88BF-AA168CC7DAC9}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H194" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{44A9303A-88D5-4BB8-9879-72F5FB7F39F1}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H195" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{09306D4D-E8BF-4998-9564-E7BA359D5135}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H196" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{515314A8-BFD2-41C1-90E5-88B3BF915352}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="B197" dT="2023-09-27T21:52:50.68" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{EBE5ABD0-D0E0-4D98-8775-45A40346A5B8}">
+    <text>757600:757619 canceled due to mistype</text>
+  </threadedComment>
+  <threadedComment ref="H197" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{45EB5FC7-B067-4E16-BC88-2FE18DB32EE9}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H198" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{D7E8C1D8-0A1A-4552-9BE2-DF2C70622C4F}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H199" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{A6232F6B-D4D4-4C06-A077-77622943784A}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H200" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{202159C9-01FE-40D8-BC35-E4387FDA6974}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H201" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{48FED36A-64A0-4E6E-B2FC-4DCB941E833D}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H202" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{98B014DF-78D4-4975-90B9-78901C25281F}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H203" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{68770FB5-ABB7-45E1-969B-1AB4920C0364}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H205" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{96A288A9-00D2-44F1-81EB-075B4A2B779B}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H206" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{70261BF8-3B60-447F-82FE-F3F6F24265EF}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H207" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{D4B85581-504C-45FC-83BB-050D16433043}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
+  <threadedComment ref="H208" dT="2023-05-02T16:25:06.05" personId="{84F4058D-3156-4278-BCDB-0417AD55C0CC}" id="{0CC2D386-04EA-4FB3-8FC0-C44B9D3B579B}">
+    <text>A = 1 mig per gen
+b= 100 @ y=151
+c= 25 @y=151,165,181,195
+d= 1 mig wheny &gt;= edyr + dur+1
+e= 100 @ y=125
+f= 25 @ y=125, 140, 155, 170</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB208"/>
+  <dimension ref="A1:AB258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B160" sqref="B160"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" customWidth="1"/>
@@ -13992,7 +15220,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="161" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>478</v>
       </c>
@@ -14069,7 +15297,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="162" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>482</v>
       </c>
@@ -14146,7 +15374,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="163" spans="2:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B163" s="22" t="s">
         <v>481</v>
       </c>
@@ -14223,7 +15451,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="164" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>484</v>
       </c>
@@ -14300,7 +15528,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="165" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
         <v>486</v>
       </c>
@@ -14377,177 +15605,3245 @@
         <v>384</v>
       </c>
     </row>
-    <row r="170" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="167" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>490</v>
+      </c>
+      <c r="B167" t="s">
+        <v>491</v>
+      </c>
+      <c r="C167" t="s">
+        <v>487</v>
+      </c>
+      <c r="D167" t="s">
+        <v>16</v>
+      </c>
+      <c r="E167" t="s">
+        <v>16</v>
+      </c>
+      <c r="F167" t="s">
+        <v>16</v>
+      </c>
+      <c r="G167" t="s">
+        <v>16</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0.05</v>
+      </c>
+      <c r="J167">
+        <v>0.05</v>
+      </c>
+      <c r="K167">
+        <v>1</v>
+      </c>
+      <c r="L167">
+        <v>300</v>
+      </c>
+      <c r="M167">
+        <v>1000</v>
+      </c>
+      <c r="N167">
+        <v>1000</v>
+      </c>
+      <c r="O167">
+        <v>10</v>
+      </c>
+      <c r="P167">
+        <v>40</v>
+      </c>
+      <c r="Q167">
+        <v>9</v>
+      </c>
+      <c r="R167">
+        <v>2</v>
+      </c>
+      <c r="S167">
+        <v>1</v>
+      </c>
+      <c r="T167">
+        <v>350</v>
+      </c>
+      <c r="U167">
+        <v>1</v>
+      </c>
+      <c r="W167">
+        <v>100</v>
+      </c>
+      <c r="X167">
+        <v>0</v>
+      </c>
+      <c r="Y167" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z167" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA167" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="168" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B168" t="s">
+        <v>492</v>
+      </c>
+      <c r="C168" t="s">
+        <v>488</v>
+      </c>
+      <c r="D168" t="s">
+        <v>16</v>
+      </c>
+      <c r="E168" t="s">
+        <v>16</v>
+      </c>
+      <c r="F168" t="s">
+        <v>16</v>
+      </c>
+      <c r="G168" t="s">
+        <v>16</v>
+      </c>
+      <c r="H168" t="s">
+        <v>296</v>
+      </c>
+      <c r="I168">
+        <v>0.05</v>
+      </c>
+      <c r="J168">
+        <v>0.05</v>
+      </c>
+      <c r="K168">
+        <v>1</v>
+      </c>
+      <c r="L168">
+        <v>300</v>
+      </c>
+      <c r="M168">
+        <v>1000</v>
+      </c>
+      <c r="N168">
+        <v>1000</v>
+      </c>
+      <c r="O168">
+        <v>10</v>
+      </c>
+      <c r="P168">
+        <v>40</v>
+      </c>
+      <c r="Q168">
+        <v>9</v>
+      </c>
+      <c r="R168">
+        <v>2</v>
+      </c>
+      <c r="S168">
+        <v>1</v>
+      </c>
+      <c r="T168">
+        <v>350</v>
+      </c>
+      <c r="U168">
+        <v>1</v>
+      </c>
+      <c r="W168">
+        <v>100</v>
+      </c>
+      <c r="X168">
+        <v>0</v>
+      </c>
+      <c r="Y168" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z168" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA168" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="169" spans="1:27" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="34" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="170" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>495</v>
+      </c>
       <c r="C170" t="s">
+        <v>493</v>
+      </c>
+      <c r="D170" t="s">
+        <v>16</v>
+      </c>
+      <c r="E170" t="s">
+        <v>16</v>
+      </c>
+      <c r="F170" t="s">
+        <v>16</v>
+      </c>
+      <c r="G170" t="s">
+        <v>16</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>0.05</v>
+      </c>
+      <c r="J170">
+        <v>0.05</v>
+      </c>
+      <c r="K170">
+        <v>5</v>
+      </c>
+      <c r="L170">
+        <v>300</v>
+      </c>
+      <c r="M170">
+        <v>1000</v>
+      </c>
+      <c r="N170">
+        <v>1000</v>
+      </c>
+      <c r="O170">
+        <v>10</v>
+      </c>
+      <c r="P170">
+        <v>40</v>
+      </c>
+      <c r="Q170">
+        <v>9</v>
+      </c>
+      <c r="R170">
+        <v>2</v>
+      </c>
+      <c r="S170">
+        <v>1</v>
+      </c>
+      <c r="T170">
+        <v>350</v>
+      </c>
+      <c r="U170">
+        <v>1</v>
+      </c>
+      <c r="W170">
+        <v>100</v>
+      </c>
+      <c r="X170">
+        <v>0</v>
+      </c>
+      <c r="Y170" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z170" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA170" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="171" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>496</v>
+      </c>
+      <c r="C171" t="s">
+        <v>497</v>
+      </c>
+      <c r="D171" t="s">
+        <v>16</v>
+      </c>
+      <c r="E171" t="s">
+        <v>16</v>
+      </c>
+      <c r="F171" t="s">
+        <v>16</v>
+      </c>
+      <c r="G171" t="s">
+        <v>16</v>
+      </c>
+      <c r="H171" t="s">
+        <v>296</v>
+      </c>
+      <c r="I171">
+        <v>0.05</v>
+      </c>
+      <c r="J171">
+        <v>0.05</v>
+      </c>
+      <c r="K171">
+        <v>5</v>
+      </c>
+      <c r="L171">
+        <v>300</v>
+      </c>
+      <c r="M171">
+        <v>1000</v>
+      </c>
+      <c r="N171">
+        <v>1000</v>
+      </c>
+      <c r="O171">
+        <v>10</v>
+      </c>
+      <c r="P171">
+        <v>40</v>
+      </c>
+      <c r="Q171">
+        <v>9</v>
+      </c>
+      <c r="R171">
+        <v>2</v>
+      </c>
+      <c r="S171">
+        <v>1</v>
+      </c>
+      <c r="T171">
+        <v>350</v>
+      </c>
+      <c r="U171">
+        <v>1</v>
+      </c>
+      <c r="W171">
+        <v>100</v>
+      </c>
+      <c r="X171">
+        <v>0</v>
+      </c>
+      <c r="Y171" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z171" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA171" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="172" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>499</v>
+      </c>
+      <c r="C172" t="s">
+        <v>498</v>
+      </c>
+      <c r="D172" t="s">
+        <v>16</v>
+      </c>
+      <c r="E172" t="s">
+        <v>16</v>
+      </c>
+      <c r="F172" t="s">
+        <v>16</v>
+      </c>
+      <c r="G172" t="s">
+        <v>16</v>
+      </c>
+      <c r="H172" t="s">
+        <v>414</v>
+      </c>
+      <c r="I172">
+        <v>0.05</v>
+      </c>
+      <c r="J172">
+        <v>0.05</v>
+      </c>
+      <c r="K172">
+        <v>5</v>
+      </c>
+      <c r="L172">
+        <v>300</v>
+      </c>
+      <c r="M172">
+        <v>1000</v>
+      </c>
+      <c r="N172">
+        <v>1000</v>
+      </c>
+      <c r="O172">
+        <v>10</v>
+      </c>
+      <c r="P172">
+        <v>40</v>
+      </c>
+      <c r="Q172">
+        <v>9</v>
+      </c>
+      <c r="R172">
+        <v>2</v>
+      </c>
+      <c r="S172">
+        <v>1</v>
+      </c>
+      <c r="T172">
+        <v>350</v>
+      </c>
+      <c r="U172">
+        <v>1</v>
+      </c>
+      <c r="W172">
+        <v>100</v>
+      </c>
+      <c r="X172">
+        <v>0</v>
+      </c>
+      <c r="Y172" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z172" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA172" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="173" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>503</v>
+      </c>
+      <c r="C173" t="s">
+        <v>500</v>
+      </c>
+      <c r="D173" t="s">
+        <v>16</v>
+      </c>
+      <c r="E173" t="s">
+        <v>16</v>
+      </c>
+      <c r="F173" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" t="s">
+        <v>16</v>
+      </c>
+      <c r="H173" t="s">
+        <v>409</v>
+      </c>
+      <c r="I173">
+        <v>0.05</v>
+      </c>
+      <c r="J173">
+        <v>0.05</v>
+      </c>
+      <c r="K173">
+        <v>5</v>
+      </c>
+      <c r="L173">
+        <v>300</v>
+      </c>
+      <c r="M173">
+        <v>1000</v>
+      </c>
+      <c r="N173">
+        <v>1000</v>
+      </c>
+      <c r="O173">
+        <v>10</v>
+      </c>
+      <c r="P173">
+        <v>40</v>
+      </c>
+      <c r="Q173">
+        <v>9</v>
+      </c>
+      <c r="R173">
+        <v>2</v>
+      </c>
+      <c r="S173">
+        <v>1</v>
+      </c>
+      <c r="T173">
+        <v>350</v>
+      </c>
+      <c r="U173">
+        <v>1</v>
+      </c>
+      <c r="W173">
+        <v>100</v>
+      </c>
+      <c r="X173">
+        <v>0</v>
+      </c>
+      <c r="Y173" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z173" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA173" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="174" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>504</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="D174" t="s">
+        <v>16</v>
+      </c>
+      <c r="E174" t="s">
+        <v>16</v>
+      </c>
+      <c r="F174" t="s">
+        <v>16</v>
+      </c>
+      <c r="G174" t="s">
+        <v>16</v>
+      </c>
+      <c r="H174" t="s">
+        <v>407</v>
+      </c>
+      <c r="I174">
+        <v>0.05</v>
+      </c>
+      <c r="J174">
+        <v>0.05</v>
+      </c>
+      <c r="K174">
+        <v>5</v>
+      </c>
+      <c r="L174">
+        <v>300</v>
+      </c>
+      <c r="M174">
+        <v>1000</v>
+      </c>
+      <c r="N174">
+        <v>1000</v>
+      </c>
+      <c r="O174">
+        <v>10</v>
+      </c>
+      <c r="P174">
+        <v>40</v>
+      </c>
+      <c r="Q174">
+        <v>9</v>
+      </c>
+      <c r="R174">
+        <v>2</v>
+      </c>
+      <c r="S174">
+        <v>1</v>
+      </c>
+      <c r="T174">
+        <v>350</v>
+      </c>
+      <c r="U174">
+        <v>1</v>
+      </c>
+      <c r="W174">
+        <v>100</v>
+      </c>
+      <c r="X174">
+        <v>0</v>
+      </c>
+      <c r="Y174" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z174" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA174" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="175" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>505</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="D175" t="s">
+        <v>16</v>
+      </c>
+      <c r="E175" t="s">
+        <v>16</v>
+      </c>
+      <c r="F175" t="s">
+        <v>16</v>
+      </c>
+      <c r="G175" t="s">
+        <v>16</v>
+      </c>
+      <c r="H175" t="s">
+        <v>403</v>
+      </c>
+      <c r="I175">
+        <v>0.05</v>
+      </c>
+      <c r="J175">
+        <v>0.05</v>
+      </c>
+      <c r="K175">
+        <v>5</v>
+      </c>
+      <c r="L175">
+        <v>300</v>
+      </c>
+      <c r="M175">
+        <v>1000</v>
+      </c>
+      <c r="N175">
+        <v>1000</v>
+      </c>
+      <c r="O175">
+        <v>10</v>
+      </c>
+      <c r="P175">
+        <v>40</v>
+      </c>
+      <c r="Q175">
+        <v>9</v>
+      </c>
+      <c r="R175">
+        <v>2</v>
+      </c>
+      <c r="S175">
+        <v>1</v>
+      </c>
+      <c r="T175">
+        <v>350</v>
+      </c>
+      <c r="U175">
+        <v>1</v>
+      </c>
+      <c r="W175">
+        <v>100</v>
+      </c>
+      <c r="X175">
+        <v>0</v>
+      </c>
+      <c r="Y175" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z175" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA175" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="176" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C176" s="29" t="s">
+        <v>506</v>
+      </c>
+      <c r="D176" t="s">
+        <v>16</v>
+      </c>
+      <c r="E176" t="s">
+        <v>16</v>
+      </c>
+      <c r="F176" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" t="s">
+        <v>16</v>
+      </c>
+      <c r="H176" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="I176" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J176" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K176" s="22">
+        <v>5</v>
+      </c>
+      <c r="L176" s="22">
+        <v>300</v>
+      </c>
+      <c r="M176" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N176" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O176" s="22">
+        <v>10</v>
+      </c>
+      <c r="P176" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q176" s="22">
+        <v>9</v>
+      </c>
+      <c r="R176" s="22">
+        <v>2</v>
+      </c>
+      <c r="S176" s="22">
+        <v>1</v>
+      </c>
+      <c r="T176" s="22">
+        <v>350</v>
+      </c>
+      <c r="U176" s="22">
+        <v>1</v>
+      </c>
+      <c r="W176" s="22">
+        <v>100</v>
+      </c>
+      <c r="X176" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y176" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z176" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA176" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="177" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>510</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="D177" t="s">
+        <v>16</v>
+      </c>
+      <c r="E177" t="s">
+        <v>16</v>
+      </c>
+      <c r="F177" t="s">
+        <v>16</v>
+      </c>
+      <c r="G177" t="s">
+        <v>16</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>0.4</v>
+      </c>
+      <c r="J177">
+        <v>0.4</v>
+      </c>
+      <c r="K177">
+        <v>5</v>
+      </c>
+      <c r="L177">
+        <v>300</v>
+      </c>
+      <c r="M177">
+        <v>1000</v>
+      </c>
+      <c r="N177">
+        <v>1000</v>
+      </c>
+      <c r="O177">
+        <v>10</v>
+      </c>
+      <c r="P177">
+        <v>40</v>
+      </c>
+      <c r="Q177">
+        <v>9</v>
+      </c>
+      <c r="R177">
+        <v>2</v>
+      </c>
+      <c r="S177">
+        <v>1</v>
+      </c>
+      <c r="T177">
+        <v>350</v>
+      </c>
+      <c r="U177">
+        <v>1</v>
+      </c>
+      <c r="W177">
+        <v>100</v>
+      </c>
+      <c r="X177">
+        <v>0</v>
+      </c>
+      <c r="Y177" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z177" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA177" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="178" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>511</v>
+      </c>
+      <c r="C178" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="D178" t="s">
+        <v>16</v>
+      </c>
+      <c r="E178" t="s">
+        <v>16</v>
+      </c>
+      <c r="F178" t="s">
+        <v>16</v>
+      </c>
+      <c r="G178" t="s">
+        <v>16</v>
+      </c>
+      <c r="H178" t="s">
+        <v>296</v>
+      </c>
+      <c r="I178">
+        <v>0.4</v>
+      </c>
+      <c r="J178">
+        <v>0.4</v>
+      </c>
+      <c r="K178">
+        <v>5</v>
+      </c>
+      <c r="L178">
+        <v>300</v>
+      </c>
+      <c r="M178">
+        <v>1000</v>
+      </c>
+      <c r="N178">
+        <v>1000</v>
+      </c>
+      <c r="O178">
+        <v>10</v>
+      </c>
+      <c r="P178">
+        <v>40</v>
+      </c>
+      <c r="Q178">
+        <v>9</v>
+      </c>
+      <c r="R178">
+        <v>2</v>
+      </c>
+      <c r="S178">
+        <v>1</v>
+      </c>
+      <c r="T178">
+        <v>350</v>
+      </c>
+      <c r="U178">
+        <v>1</v>
+      </c>
+      <c r="W178">
+        <v>100</v>
+      </c>
+      <c r="X178">
+        <v>0</v>
+      </c>
+      <c r="Y178" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z178" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA178" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B179" t="s">
+        <v>517</v>
+      </c>
+      <c r="C179" s="36" t="s">
+        <v>512</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0.4</v>
+      </c>
+      <c r="J179">
+        <v>0.05</v>
+      </c>
+      <c r="K179">
+        <v>5</v>
+      </c>
+      <c r="L179">
+        <v>300</v>
+      </c>
+      <c r="M179">
+        <v>1000</v>
+      </c>
+      <c r="N179">
+        <v>1000</v>
+      </c>
+      <c r="O179">
+        <v>10</v>
+      </c>
+      <c r="P179">
+        <v>40</v>
+      </c>
+      <c r="Q179">
+        <v>9</v>
+      </c>
+      <c r="R179">
+        <v>2</v>
+      </c>
+      <c r="S179">
+        <v>1</v>
+      </c>
+      <c r="T179">
+        <v>350</v>
+      </c>
+      <c r="U179">
+        <v>1</v>
+      </c>
+      <c r="W179">
+        <v>100</v>
+      </c>
+      <c r="X179">
+        <v>0</v>
+      </c>
+      <c r="Y179" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z179" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA179" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="180" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>516</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="H180" t="s">
+        <v>296</v>
+      </c>
+      <c r="I180">
+        <v>0.4</v>
+      </c>
+      <c r="J180">
+        <v>0.05</v>
+      </c>
+      <c r="K180">
+        <v>5</v>
+      </c>
+      <c r="L180">
+        <v>300</v>
+      </c>
+      <c r="M180">
+        <v>1000</v>
+      </c>
+      <c r="N180">
+        <v>1000</v>
+      </c>
+      <c r="O180">
+        <v>10</v>
+      </c>
+      <c r="P180">
+        <v>40</v>
+      </c>
+      <c r="Q180">
+        <v>9</v>
+      </c>
+      <c r="R180">
+        <v>2</v>
+      </c>
+      <c r="S180">
+        <v>1</v>
+      </c>
+      <c r="T180">
+        <v>350</v>
+      </c>
+      <c r="U180">
+        <v>1</v>
+      </c>
+      <c r="W180">
+        <v>100</v>
+      </c>
+      <c r="X180">
+        <v>0</v>
+      </c>
+      <c r="Y180" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z180" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA180" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="181" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>518</v>
+      </c>
+      <c r="C181" s="36" t="s">
+        <v>514</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>0.05</v>
+      </c>
+      <c r="J181">
+        <v>0.4</v>
+      </c>
+      <c r="K181">
+        <v>5</v>
+      </c>
+      <c r="L181">
+        <v>300</v>
+      </c>
+      <c r="M181">
+        <v>1000</v>
+      </c>
+      <c r="N181">
+        <v>1000</v>
+      </c>
+      <c r="O181">
+        <v>10</v>
+      </c>
+      <c r="P181">
+        <v>40</v>
+      </c>
+      <c r="Q181">
+        <v>9</v>
+      </c>
+      <c r="R181">
+        <v>2</v>
+      </c>
+      <c r="S181">
+        <v>1</v>
+      </c>
+      <c r="T181">
+        <v>350</v>
+      </c>
+      <c r="U181">
+        <v>1</v>
+      </c>
+      <c r="W181">
+        <v>100</v>
+      </c>
+      <c r="X181">
+        <v>0</v>
+      </c>
+      <c r="Y181" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z181" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA181" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="182" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="C182" s="35" t="s">
+        <v>515</v>
+      </c>
+      <c r="H182" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="I182" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J182" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="K182" s="22">
+        <v>5</v>
+      </c>
+      <c r="L182" s="22">
+        <v>300</v>
+      </c>
+      <c r="M182" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N182" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O182" s="22">
+        <v>10</v>
+      </c>
+      <c r="P182" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q182" s="22">
+        <v>9</v>
+      </c>
+      <c r="R182" s="22">
+        <v>2</v>
+      </c>
+      <c r="S182" s="22">
+        <v>1</v>
+      </c>
+      <c r="T182" s="22">
+        <v>350</v>
+      </c>
+      <c r="U182" s="22">
+        <v>1</v>
+      </c>
+      <c r="W182" s="22">
+        <v>100</v>
+      </c>
+      <c r="X182" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y182" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z182" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA182" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="183" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>589</v>
+      </c>
+      <c r="B183" t="s">
+        <v>524</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="D183" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="E183" s="26"/>
+      <c r="F183" s="26"/>
+      <c r="G183" s="26"/>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>0.05</v>
+      </c>
+      <c r="J183">
+        <v>0.05</v>
+      </c>
+      <c r="K183">
+        <v>5</v>
+      </c>
+      <c r="L183">
+        <v>100</v>
+      </c>
+      <c r="M183">
+        <v>1000</v>
+      </c>
+      <c r="N183">
+        <v>1000</v>
+      </c>
+      <c r="O183">
+        <v>10</v>
+      </c>
+      <c r="P183">
+        <v>40</v>
+      </c>
+      <c r="Q183">
+        <v>9</v>
+      </c>
+      <c r="R183">
+        <v>2</v>
+      </c>
+      <c r="S183">
+        <v>1</v>
+      </c>
+      <c r="T183">
+        <v>350</v>
+      </c>
+      <c r="U183">
+        <v>1</v>
+      </c>
+      <c r="W183">
+        <v>100</v>
+      </c>
+      <c r="X183">
+        <v>0</v>
+      </c>
+      <c r="Y183" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z183" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA183" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="184" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>525</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="D184" t="s">
+        <v>16</v>
+      </c>
+      <c r="E184" t="s">
+        <v>16</v>
+      </c>
+      <c r="F184" t="s">
+        <v>16</v>
+      </c>
+      <c r="G184" t="s">
+        <v>16</v>
+      </c>
+      <c r="H184" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="I184">
+        <v>0.05</v>
+      </c>
+      <c r="J184">
+        <v>0.05</v>
+      </c>
+      <c r="K184">
+        <v>5</v>
+      </c>
+      <c r="L184">
+        <v>100</v>
+      </c>
+      <c r="M184">
+        <v>1000</v>
+      </c>
+      <c r="N184">
+        <v>1000</v>
+      </c>
+      <c r="O184">
+        <v>10</v>
+      </c>
+      <c r="P184">
+        <v>40</v>
+      </c>
+      <c r="Q184">
+        <v>9</v>
+      </c>
+      <c r="R184">
+        <v>2</v>
+      </c>
+      <c r="S184">
+        <v>1</v>
+      </c>
+      <c r="T184">
+        <v>350</v>
+      </c>
+      <c r="U184">
+        <v>1</v>
+      </c>
+      <c r="W184">
+        <v>100</v>
+      </c>
+      <c r="X184">
+        <v>0</v>
+      </c>
+      <c r="Y184" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z184" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA184" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="185" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>590</v>
+      </c>
+      <c r="B185" t="s">
+        <v>527</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="D185" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="E185" s="26"/>
+      <c r="F185" s="26"/>
+      <c r="G185" s="26"/>
+      <c r="H185" t="s">
+        <v>414</v>
+      </c>
+      <c r="I185">
+        <v>0.05</v>
+      </c>
+      <c r="J185">
+        <v>0.05</v>
+      </c>
+      <c r="K185">
+        <v>5</v>
+      </c>
+      <c r="L185">
+        <v>100</v>
+      </c>
+      <c r="M185">
+        <v>1000</v>
+      </c>
+      <c r="N185">
+        <v>1000</v>
+      </c>
+      <c r="O185">
+        <v>10</v>
+      </c>
+      <c r="P185">
+        <v>40</v>
+      </c>
+      <c r="Q185">
+        <v>9</v>
+      </c>
+      <c r="R185">
+        <v>2</v>
+      </c>
+      <c r="S185">
+        <v>1</v>
+      </c>
+      <c r="T185">
+        <v>350</v>
+      </c>
+      <c r="U185">
+        <v>1</v>
+      </c>
+      <c r="W185">
+        <v>100</v>
+      </c>
+      <c r="X185">
+        <v>0</v>
+      </c>
+      <c r="Y185" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z185" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA185" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="186" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="B186" s="22" t="s">
+        <v>526</v>
+      </c>
+      <c r="C186" s="29" t="s">
+        <v>523</v>
+      </c>
+      <c r="D186" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="E186" s="30"/>
+      <c r="F186" s="30"/>
+      <c r="G186" s="30"/>
+      <c r="H186" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="I186" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J186" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K186" s="22">
+        <v>5</v>
+      </c>
+      <c r="L186" s="22">
+        <v>100</v>
+      </c>
+      <c r="M186" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N186" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O186" s="22">
+        <v>10</v>
+      </c>
+      <c r="P186" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q186" s="22">
+        <v>9</v>
+      </c>
+      <c r="R186" s="22">
+        <v>2</v>
+      </c>
+      <c r="S186" s="22">
+        <v>1</v>
+      </c>
+      <c r="T186" s="22">
+        <v>350</v>
+      </c>
+      <c r="U186" s="22">
+        <v>1</v>
+      </c>
+      <c r="W186" s="22">
+        <v>100</v>
+      </c>
+      <c r="X186" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y186" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z186" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA186" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="187" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B187" t="s">
+        <v>532</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="D187" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E187" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F187" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G187" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>0.05</v>
+      </c>
+      <c r="J187">
+        <v>0.05</v>
+      </c>
+      <c r="K187">
+        <v>5</v>
+      </c>
+      <c r="L187">
+        <v>700</v>
+      </c>
+      <c r="M187">
+        <v>1000</v>
+      </c>
+      <c r="N187">
+        <v>1000</v>
+      </c>
+      <c r="O187">
+        <v>10</v>
+      </c>
+      <c r="P187">
+        <v>40</v>
+      </c>
+      <c r="Q187">
+        <v>9</v>
+      </c>
+      <c r="R187">
+        <v>2</v>
+      </c>
+      <c r="S187">
+        <v>1</v>
+      </c>
+      <c r="T187">
+        <v>350</v>
+      </c>
+      <c r="U187">
+        <v>1</v>
+      </c>
+      <c r="W187">
+        <v>100</v>
+      </c>
+      <c r="X187">
+        <v>0</v>
+      </c>
+      <c r="Y187" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z187" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA187" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="188" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B188" t="s">
+        <v>533</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="D188" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E188" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F188" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G188" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H188" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="I188">
+        <v>0.05</v>
+      </c>
+      <c r="J188">
+        <v>0.05</v>
+      </c>
+      <c r="K188">
+        <v>5</v>
+      </c>
+      <c r="L188">
+        <v>700</v>
+      </c>
+      <c r="M188">
+        <v>1000</v>
+      </c>
+      <c r="N188">
+        <v>1000</v>
+      </c>
+      <c r="O188">
+        <v>10</v>
+      </c>
+      <c r="P188">
+        <v>40</v>
+      </c>
+      <c r="Q188">
+        <v>9</v>
+      </c>
+      <c r="R188">
+        <v>2</v>
+      </c>
+      <c r="S188">
+        <v>1</v>
+      </c>
+      <c r="T188">
+        <v>350</v>
+      </c>
+      <c r="U188">
+        <v>1</v>
+      </c>
+      <c r="W188">
+        <v>100</v>
+      </c>
+      <c r="X188">
+        <v>0</v>
+      </c>
+      <c r="Y188" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z188" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA188" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="189" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B189" t="s">
+        <v>534</v>
+      </c>
+      <c r="C189" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="D189" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E189" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F189" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G189" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H189" t="s">
+        <v>414</v>
+      </c>
+      <c r="I189">
+        <v>0.05</v>
+      </c>
+      <c r="J189">
+        <v>0.05</v>
+      </c>
+      <c r="K189">
+        <v>5</v>
+      </c>
+      <c r="L189">
+        <v>700</v>
+      </c>
+      <c r="M189">
+        <v>1000</v>
+      </c>
+      <c r="N189">
+        <v>1000</v>
+      </c>
+      <c r="O189">
+        <v>10</v>
+      </c>
+      <c r="P189">
+        <v>40</v>
+      </c>
+      <c r="Q189">
+        <v>9</v>
+      </c>
+      <c r="R189">
+        <v>2</v>
+      </c>
+      <c r="S189">
+        <v>1</v>
+      </c>
+      <c r="T189">
+        <v>350</v>
+      </c>
+      <c r="U189">
+        <v>1</v>
+      </c>
+      <c r="W189">
+        <v>100</v>
+      </c>
+      <c r="X189">
+        <v>0</v>
+      </c>
+      <c r="Y189" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z189" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA189" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="190" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="C190" s="29" t="s">
+        <v>531</v>
+      </c>
+      <c r="D190" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E190" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F190" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G190" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H190" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="I190" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J190" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K190" s="22">
+        <v>5</v>
+      </c>
+      <c r="L190" s="22">
+        <v>700</v>
+      </c>
+      <c r="M190" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N190" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O190" s="22">
+        <v>10</v>
+      </c>
+      <c r="P190" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q190" s="22">
+        <v>9</v>
+      </c>
+      <c r="R190" s="22">
+        <v>2</v>
+      </c>
+      <c r="S190" s="22">
+        <v>1</v>
+      </c>
+      <c r="T190" s="22">
+        <v>350</v>
+      </c>
+      <c r="U190" s="22">
+        <v>1</v>
+      </c>
+      <c r="W190" s="22">
+        <v>100</v>
+      </c>
+      <c r="X190" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y190" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z190" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA190" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="191" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B191" t="s">
+        <v>538</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="D191" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E191" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F191" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G191" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H191" t="s">
+        <v>296</v>
+      </c>
+      <c r="I191">
+        <v>0.05</v>
+      </c>
+      <c r="J191">
+        <v>0.05</v>
+      </c>
+      <c r="K191">
+        <v>5</v>
+      </c>
+      <c r="L191" t="s">
+        <v>465</v>
+      </c>
+      <c r="M191">
+        <v>1000</v>
+      </c>
+      <c r="N191">
+        <v>1000</v>
+      </c>
+      <c r="O191" t="s">
+        <v>463</v>
+      </c>
+      <c r="P191" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q191">
+        <v>9</v>
+      </c>
+      <c r="R191">
+        <v>2</v>
+      </c>
+      <c r="S191">
+        <v>1</v>
+      </c>
+      <c r="T191">
+        <v>350</v>
+      </c>
+      <c r="U191">
+        <v>1</v>
+      </c>
+      <c r="W191">
+        <v>100</v>
+      </c>
+      <c r="X191">
+        <v>0</v>
+      </c>
+      <c r="Y191" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z191" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA191" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB191" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="192" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="C192" s="29" t="s">
+        <v>537</v>
+      </c>
+      <c r="D192" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E192" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F192" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G192" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H192" s="22">
+        <v>0</v>
+      </c>
+      <c r="I192" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J192" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K192" s="22">
+        <v>5</v>
+      </c>
+      <c r="L192" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="M192" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N192" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O192" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="P192" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q192" s="22">
+        <v>9</v>
+      </c>
+      <c r="R192" s="22">
+        <v>2</v>
+      </c>
+      <c r="S192" s="22">
+        <v>1</v>
+      </c>
+      <c r="T192" s="22">
+        <v>350</v>
+      </c>
+      <c r="U192" s="22">
+        <v>1</v>
+      </c>
+      <c r="W192" s="22">
+        <v>100</v>
+      </c>
+      <c r="X192" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y192" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z192" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA192" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="AB192" s="22" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>543</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="D193" t="s">
+        <v>16</v>
+      </c>
+      <c r="E193" t="s">
+        <v>16</v>
+      </c>
+      <c r="F193" t="s">
+        <v>16</v>
+      </c>
+      <c r="G193" t="s">
+        <v>16</v>
+      </c>
+      <c r="H193" t="s">
+        <v>409</v>
+      </c>
+      <c r="I193">
+        <v>0.05</v>
+      </c>
+      <c r="J193">
+        <v>0.05</v>
+      </c>
+      <c r="K193">
+        <v>5</v>
+      </c>
+      <c r="L193">
+        <v>300</v>
+      </c>
+      <c r="M193">
+        <v>1000</v>
+      </c>
+      <c r="N193">
+        <v>1000</v>
+      </c>
+      <c r="O193">
+        <v>10</v>
+      </c>
+      <c r="P193">
+        <v>40</v>
+      </c>
+      <c r="Q193">
+        <v>9</v>
+      </c>
+      <c r="R193">
+        <v>2</v>
+      </c>
+      <c r="S193">
+        <v>1</v>
+      </c>
+      <c r="T193">
+        <v>350</v>
+      </c>
+      <c r="U193">
+        <v>1</v>
+      </c>
+      <c r="W193">
+        <v>100</v>
+      </c>
+      <c r="X193">
+        <v>0</v>
+      </c>
+      <c r="Y193" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z193" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>542</v>
+      </c>
+      <c r="C194" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="D194" t="s">
+        <v>16</v>
+      </c>
+      <c r="E194" t="s">
+        <v>16</v>
+      </c>
+      <c r="F194" t="s">
+        <v>16</v>
+      </c>
+      <c r="G194" t="s">
+        <v>16</v>
+      </c>
+      <c r="H194" t="s">
+        <v>414</v>
+      </c>
+      <c r="I194">
+        <v>0.05</v>
+      </c>
+      <c r="J194">
+        <v>0.05</v>
+      </c>
+      <c r="K194">
+        <v>5</v>
+      </c>
+      <c r="L194">
+        <v>300</v>
+      </c>
+      <c r="M194">
+        <v>1000</v>
+      </c>
+      <c r="N194">
+        <v>1000</v>
+      </c>
+      <c r="O194">
+        <v>10</v>
+      </c>
+      <c r="P194">
+        <v>40</v>
+      </c>
+      <c r="Q194">
+        <v>9</v>
+      </c>
+      <c r="R194">
+        <v>2</v>
+      </c>
+      <c r="S194">
+        <v>1</v>
+      </c>
+      <c r="T194">
+        <v>350</v>
+      </c>
+      <c r="U194">
+        <v>1</v>
+      </c>
+      <c r="W194">
+        <v>100</v>
+      </c>
+      <c r="X194">
+        <v>0</v>
+      </c>
+      <c r="Y194" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z194" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA194" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="195" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>541</v>
+      </c>
+      <c r="C195" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="D195" t="s">
+        <v>16</v>
+      </c>
+      <c r="E195" t="s">
+        <v>16</v>
+      </c>
+      <c r="F195" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" t="s">
+        <v>16</v>
+      </c>
+      <c r="H195" t="s">
+        <v>296</v>
+      </c>
+      <c r="I195">
+        <v>0.05</v>
+      </c>
+      <c r="J195">
+        <v>0.05</v>
+      </c>
+      <c r="K195">
+        <v>5</v>
+      </c>
+      <c r="L195">
+        <v>300</v>
+      </c>
+      <c r="M195">
+        <v>1000</v>
+      </c>
+      <c r="N195">
+        <v>1000</v>
+      </c>
+      <c r="O195">
+        <v>10</v>
+      </c>
+      <c r="P195">
+        <v>40</v>
+      </c>
+      <c r="Q195">
+        <v>9</v>
+      </c>
+      <c r="R195">
+        <v>2</v>
+      </c>
+      <c r="S195">
+        <v>1</v>
+      </c>
+      <c r="T195">
+        <v>350</v>
+      </c>
+      <c r="U195">
+        <v>1</v>
+      </c>
+      <c r="W195">
+        <v>100</v>
+      </c>
+      <c r="X195">
+        <v>0</v>
+      </c>
+      <c r="Y195" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z195" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA195" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="196" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="C196" s="29" t="s">
+        <v>547</v>
+      </c>
+      <c r="D196" t="s">
+        <v>16</v>
+      </c>
+      <c r="E196" t="s">
+        <v>16</v>
+      </c>
+      <c r="F196" t="s">
+        <v>16</v>
+      </c>
+      <c r="G196" t="s">
+        <v>16</v>
+      </c>
+      <c r="H196" s="22">
+        <v>0</v>
+      </c>
+      <c r="I196" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J196" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K196" s="22">
+        <v>5</v>
+      </c>
+      <c r="L196" s="22">
+        <v>300</v>
+      </c>
+      <c r="M196" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N196" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O196" s="22">
+        <v>10</v>
+      </c>
+      <c r="P196" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q196" s="22">
+        <v>9</v>
+      </c>
+      <c r="R196" s="22">
+        <v>2</v>
+      </c>
+      <c r="S196" s="22">
+        <v>1</v>
+      </c>
+      <c r="T196" s="22">
+        <v>350</v>
+      </c>
+      <c r="U196" s="22">
+        <v>1</v>
+      </c>
+      <c r="W196" s="22">
+        <v>100</v>
+      </c>
+      <c r="X196" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y196" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z196" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA196" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="197" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>549</v>
+      </c>
+      <c r="C197" t="s">
+        <v>548</v>
+      </c>
+      <c r="D197" t="s">
+        <v>16</v>
+      </c>
+      <c r="E197" t="s">
+        <v>16</v>
+      </c>
+      <c r="F197" t="s">
+        <v>16</v>
+      </c>
+      <c r="G197" t="s">
+        <v>16</v>
+      </c>
+      <c r="H197" t="s">
+        <v>296</v>
+      </c>
+      <c r="I197">
+        <v>0.05</v>
+      </c>
+      <c r="J197">
+        <v>0.4</v>
+      </c>
+      <c r="K197">
+        <v>5</v>
+      </c>
+      <c r="L197">
+        <v>300</v>
+      </c>
+      <c r="M197">
+        <v>1000</v>
+      </c>
+      <c r="N197">
+        <v>1000</v>
+      </c>
+      <c r="O197">
+        <v>10</v>
+      </c>
+      <c r="P197">
+        <v>40</v>
+      </c>
+      <c r="Q197">
+        <v>9</v>
+      </c>
+      <c r="R197">
+        <v>2</v>
+      </c>
+      <c r="S197">
+        <v>1</v>
+      </c>
+      <c r="T197">
+        <v>350</v>
+      </c>
+      <c r="U197">
+        <v>1</v>
+      </c>
+      <c r="W197">
+        <v>100</v>
+      </c>
+      <c r="X197">
+        <v>0</v>
+      </c>
+      <c r="Y197" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z197" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA197" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="198" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>550</v>
+      </c>
+      <c r="C198" t="s">
+        <v>552</v>
+      </c>
+      <c r="D198" t="s">
+        <v>16</v>
+      </c>
+      <c r="E198" t="s">
+        <v>16</v>
+      </c>
+      <c r="F198" t="s">
+        <v>16</v>
+      </c>
+      <c r="G198" t="s">
+        <v>16</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>0.4</v>
+      </c>
+      <c r="J198">
+        <v>0.05</v>
+      </c>
+      <c r="K198">
+        <v>5</v>
+      </c>
+      <c r="L198">
+        <v>300</v>
+      </c>
+      <c r="M198">
+        <v>1000</v>
+      </c>
+      <c r="N198">
+        <v>1000</v>
+      </c>
+      <c r="O198">
+        <v>10</v>
+      </c>
+      <c r="P198">
+        <v>40</v>
+      </c>
+      <c r="Q198">
+        <v>9</v>
+      </c>
+      <c r="R198">
+        <v>2</v>
+      </c>
+      <c r="S198">
+        <v>1</v>
+      </c>
+      <c r="T198">
+        <v>350</v>
+      </c>
+      <c r="U198">
+        <v>1</v>
+      </c>
+      <c r="W198">
+        <v>100</v>
+      </c>
+      <c r="X198">
+        <v>0</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z198" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA198" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="199" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
+        <v>553</v>
+      </c>
+      <c r="C199" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <v>0.05</v>
+      </c>
+      <c r="J199">
+        <v>0.4</v>
+      </c>
+      <c r="K199">
+        <v>5</v>
+      </c>
+      <c r="L199">
+        <v>300</v>
+      </c>
+      <c r="M199">
+        <v>1000</v>
+      </c>
+      <c r="N199">
+        <v>1000</v>
+      </c>
+      <c r="O199">
+        <v>10</v>
+      </c>
+      <c r="P199">
+        <v>40</v>
+      </c>
+      <c r="Q199">
+        <v>9</v>
+      </c>
+      <c r="R199">
+        <v>2</v>
+      </c>
+      <c r="S199">
+        <v>1</v>
+      </c>
+      <c r="T199">
+        <v>350</v>
+      </c>
+      <c r="U199">
+        <v>1</v>
+      </c>
+      <c r="W199">
+        <v>100</v>
+      </c>
+      <c r="X199">
+        <v>0</v>
+      </c>
+      <c r="Y199" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z199" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA199" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="200" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="22" t="s">
+        <v>554</v>
+      </c>
+      <c r="C200" s="38" t="s">
+        <v>571</v>
+      </c>
+      <c r="D200" t="s">
+        <v>16</v>
+      </c>
+      <c r="E200" t="s">
+        <v>16</v>
+      </c>
+      <c r="F200" t="s">
+        <v>16</v>
+      </c>
+      <c r="G200" t="s">
+        <v>16</v>
+      </c>
+      <c r="H200" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="I200" s="29">
+        <v>0.4</v>
+      </c>
+      <c r="J200" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="K200" s="29">
+        <v>5</v>
+      </c>
+      <c r="L200" s="29">
+        <v>300</v>
+      </c>
+      <c r="M200" s="29">
+        <v>1000</v>
+      </c>
+      <c r="N200" s="29">
+        <v>1000</v>
+      </c>
+      <c r="O200" s="29">
+        <v>10</v>
+      </c>
+      <c r="P200" s="29">
+        <v>40</v>
+      </c>
+      <c r="Q200" s="29">
+        <v>9</v>
+      </c>
+      <c r="R200" s="29">
+        <v>2</v>
+      </c>
+      <c r="S200" s="29">
+        <v>1</v>
+      </c>
+      <c r="T200" s="29">
+        <v>350</v>
+      </c>
+      <c r="U200" s="29">
+        <v>1</v>
+      </c>
+      <c r="V200" s="29"/>
+      <c r="W200" s="29">
+        <v>100</v>
+      </c>
+      <c r="X200" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y200" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z200" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA200" s="29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="201" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>574</v>
+      </c>
+      <c r="B201" t="s">
+        <v>557</v>
+      </c>
+      <c r="C201" t="s">
+        <v>556</v>
+      </c>
+      <c r="D201" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+      <c r="I201">
+        <v>0.05</v>
+      </c>
+      <c r="J201">
+        <v>0.05</v>
+      </c>
+      <c r="K201">
+        <v>5</v>
+      </c>
+      <c r="L201">
+        <v>100</v>
+      </c>
+      <c r="M201">
+        <v>1000</v>
+      </c>
+      <c r="N201">
+        <v>1000</v>
+      </c>
+      <c r="O201">
+        <v>10</v>
+      </c>
+      <c r="P201">
+        <v>40</v>
+      </c>
+      <c r="Q201">
+        <v>9</v>
+      </c>
+      <c r="R201">
+        <v>2</v>
+      </c>
+      <c r="S201">
+        <v>1</v>
+      </c>
+      <c r="T201">
+        <v>350</v>
+      </c>
+      <c r="U201">
+        <v>1</v>
+      </c>
+      <c r="W201">
+        <v>100</v>
+      </c>
+      <c r="X201">
+        <v>0</v>
+      </c>
+      <c r="Y201" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z201" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA201" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="202" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>573</v>
+      </c>
+      <c r="B202" t="s">
+        <v>560</v>
+      </c>
+      <c r="C202" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="D202" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="E202" s="26"/>
+      <c r="F202" s="26"/>
+      <c r="G202" s="26"/>
+      <c r="H202" t="s">
+        <v>414</v>
+      </c>
+      <c r="I202">
+        <v>0.05</v>
+      </c>
+      <c r="J202">
+        <v>0.05</v>
+      </c>
+      <c r="K202">
+        <v>5</v>
+      </c>
+      <c r="L202">
+        <v>100</v>
+      </c>
+      <c r="M202">
+        <v>1000</v>
+      </c>
+      <c r="N202">
+        <v>1000</v>
+      </c>
+      <c r="O202">
+        <v>10</v>
+      </c>
+      <c r="P202">
+        <v>40</v>
+      </c>
+      <c r="Q202">
+        <v>9</v>
+      </c>
+      <c r="R202">
+        <v>2</v>
+      </c>
+      <c r="S202">
+        <v>1</v>
+      </c>
+      <c r="T202">
+        <v>350</v>
+      </c>
+      <c r="U202">
+        <v>1</v>
+      </c>
+      <c r="W202">
+        <v>100</v>
+      </c>
+      <c r="X202">
+        <v>0</v>
+      </c>
+      <c r="Y202" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z202" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA202" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="203" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="B203" s="22" t="s">
+        <v>561</v>
+      </c>
+      <c r="C203" s="29" t="s">
+        <v>559</v>
+      </c>
+      <c r="D203" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="E203" s="30"/>
+      <c r="F203" s="30"/>
+      <c r="G203" s="30"/>
+      <c r="H203" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="I203" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J203" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K203" s="22">
+        <v>5</v>
+      </c>
+      <c r="L203" s="22">
+        <v>100</v>
+      </c>
+      <c r="M203" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N203" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O203" s="22">
+        <v>10</v>
+      </c>
+      <c r="P203" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q203" s="22">
+        <v>9</v>
+      </c>
+      <c r="R203" s="22">
+        <v>2</v>
+      </c>
+      <c r="S203" s="22">
+        <v>1</v>
+      </c>
+      <c r="T203" s="22">
+        <v>350</v>
+      </c>
+      <c r="U203" s="22">
+        <v>1</v>
+      </c>
+      <c r="W203" s="22">
+        <v>100</v>
+      </c>
+      <c r="X203" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y203" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z203" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA203" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="204" spans="1:27" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="37" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="205" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B205" t="s">
+        <v>568</v>
+      </c>
+      <c r="C205" t="s">
+        <v>563</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="I205">
+        <v>0.05</v>
+      </c>
+      <c r="J205">
+        <v>0.05</v>
+      </c>
+      <c r="K205">
+        <v>5</v>
+      </c>
+      <c r="L205">
+        <v>100</v>
+      </c>
+      <c r="M205">
+        <v>1000</v>
+      </c>
+      <c r="N205">
+        <v>1000</v>
+      </c>
+      <c r="O205">
+        <v>10</v>
+      </c>
+      <c r="P205">
+        <v>40</v>
+      </c>
+      <c r="Q205">
+        <v>9</v>
+      </c>
+      <c r="R205">
+        <v>2</v>
+      </c>
+      <c r="S205">
+        <v>1</v>
+      </c>
+      <c r="T205">
+        <v>350</v>
+      </c>
+      <c r="U205">
+        <v>1</v>
+      </c>
+      <c r="W205">
+        <v>100</v>
+      </c>
+      <c r="X205">
+        <v>0</v>
+      </c>
+      <c r="Y205" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z205" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA205" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="206" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
+        <v>567</v>
+      </c>
+      <c r="C206" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="D206" s="26"/>
+      <c r="E206" s="26"/>
+      <c r="F206" s="26"/>
+      <c r="G206" s="26"/>
+      <c r="H206" t="s">
+        <v>414</v>
+      </c>
+      <c r="I206">
+        <v>0.05</v>
+      </c>
+      <c r="J206">
+        <v>0.05</v>
+      </c>
+      <c r="K206">
+        <v>5</v>
+      </c>
+      <c r="L206">
+        <v>100</v>
+      </c>
+      <c r="M206">
+        <v>1000</v>
+      </c>
+      <c r="N206">
+        <v>1000</v>
+      </c>
+      <c r="O206">
+        <v>10</v>
+      </c>
+      <c r="P206">
+        <v>40</v>
+      </c>
+      <c r="Q206">
+        <v>9</v>
+      </c>
+      <c r="R206">
+        <v>2</v>
+      </c>
+      <c r="S206">
+        <v>1</v>
+      </c>
+      <c r="T206">
+        <v>350</v>
+      </c>
+      <c r="U206">
+        <v>1</v>
+      </c>
+      <c r="W206">
+        <v>100</v>
+      </c>
+      <c r="X206">
+        <v>0</v>
+      </c>
+      <c r="Y206" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z206" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA206" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="207" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B207" t="s">
+        <v>566</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="D207" s="26"/>
+      <c r="E207" s="26"/>
+      <c r="F207" s="26"/>
+      <c r="G207" s="26"/>
+      <c r="H207" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="I207">
+        <v>0.05</v>
+      </c>
+      <c r="J207">
+        <v>0.05</v>
+      </c>
+      <c r="K207">
+        <v>5</v>
+      </c>
+      <c r="L207">
+        <v>100</v>
+      </c>
+      <c r="M207">
+        <v>1000</v>
+      </c>
+      <c r="N207">
+        <v>1000</v>
+      </c>
+      <c r="O207">
+        <v>10</v>
+      </c>
+      <c r="P207">
+        <v>40</v>
+      </c>
+      <c r="Q207">
+        <v>9</v>
+      </c>
+      <c r="R207">
+        <v>2</v>
+      </c>
+      <c r="S207">
+        <v>1</v>
+      </c>
+      <c r="T207">
+        <v>350</v>
+      </c>
+      <c r="U207">
+        <v>1</v>
+      </c>
+      <c r="W207">
+        <v>100</v>
+      </c>
+      <c r="X207">
+        <v>0</v>
+      </c>
+      <c r="Y207" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z207" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA207" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="208" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="22" t="s">
+        <v>570</v>
+      </c>
+      <c r="C208" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="H208" s="22">
+        <v>0</v>
+      </c>
+      <c r="I208" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="J208" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K208" s="22">
+        <v>5</v>
+      </c>
+      <c r="L208" s="22">
+        <v>100</v>
+      </c>
+      <c r="M208" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N208" s="22">
+        <v>1000</v>
+      </c>
+      <c r="O208" s="22">
+        <v>10</v>
+      </c>
+      <c r="P208" s="22">
+        <v>40</v>
+      </c>
+      <c r="Q208" s="22">
+        <v>9</v>
+      </c>
+      <c r="R208" s="22">
+        <v>2</v>
+      </c>
+      <c r="S208" s="22">
+        <v>1</v>
+      </c>
+      <c r="T208" s="22">
+        <v>350</v>
+      </c>
+      <c r="U208" s="22">
+        <v>1</v>
+      </c>
+      <c r="W208" s="22">
+        <v>100</v>
+      </c>
+      <c r="X208" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y208" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z208" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA208" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C220" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="171" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C171" t="s">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C221" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="172" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C172" s="21" t="s">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C222" s="21" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="173" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C173" t="s">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C223" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C177" t="s">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C227" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C179" t="s">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C229" t="s">
         <v>188</v>
       </c>
-      <c r="H179" t="s">
+      <c r="H229" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C180" t="s">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C230" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C181" s="20" t="s">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C231" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C182" t="s">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C232" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C183" t="s">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C233" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>227</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B234" t="s">
         <v>226</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C234" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C185" s="8" t="s">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C235" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C186" t="s">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C236" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C187" t="s">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C237" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C188" t="s">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C238" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C191" t="s">
+    <row r="241" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C241" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C192" t="s">
+    <row r="242" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C242" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C193" t="s">
+    <row r="243" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C243" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C194" t="s">
+    <row r="244" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C244" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C195" t="s">
+    <row r="245" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C245" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C196" t="s">
+    <row r="246" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C246" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="198" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D198" s="6" t="s">
+    <row r="248" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D248" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D199" t="s">
+    <row r="249" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D249" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="200" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D200" s="7" t="s">
+    <row r="250" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D250" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="201" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D201" s="3" t="s">
+    <row r="251" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D251" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="202" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D202" s="3" t="s">
+    <row r="252" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D252" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="203" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D203" s="3" t="s">
+    <row r="253" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D253" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="204" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D204" s="3" t="s">
+    <row r="254" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D254" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="205" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D205" s="6" t="s">
+    <row r="255" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D255" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="206" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D206" s="3" t="s">
+    <row r="256" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D256" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="208" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D208" s="3" t="s">
+    <row r="258" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D258" s="3" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C172" r:id="rId1" display="https://www.natureserve.org/sites/default/files/publications/files/natureserveconservationstatusfactors_apr12.pdf" xr:uid="{0084F411-030C-4AB0-936F-5DA9CEBDCCC8}"/>
+    <hyperlink ref="C222" r:id="rId1" display="https://www.natureserve.org/sites/default/files/publications/files/natureserveconservationstatusfactors_apr12.pdf" xr:uid="{0084F411-030C-4AB0-936F-5DA9CEBDCCC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FA6279-E689-4C49-8985-23DAA3BE3327}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>576</v>
+      </c>
+      <c r="D2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>588</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>